<commit_message>
set up ch 3 hw
</commit_message>
<xml_diff>
--- a/COMP300-HomeworkProblems-SP20.xlsx
+++ b/COMP300-HomeworkProblems-SP20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benlo\DataMining2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B731BCA9-505C-41F6-9995-034CE788445F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6B2BF9-D7B8-40D0-ADF7-1FD451562A90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HW Index" sheetId="38" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="440">
   <si>
     <t>Mean</t>
   </si>
@@ -1450,7 +1450,76 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>:")</t>
+    <t>17,17,17</t>
+  </si>
+  <si>
+    <t>22,22,22</t>
+  </si>
+  <si>
+    <t>30,30,30</t>
+  </si>
+  <si>
+    <t>34,34,34</t>
+  </si>
+  <si>
+    <t>37,37,37</t>
+  </si>
+  <si>
+    <t>46,46,46</t>
+  </si>
+  <si>
+    <t>49,49,49</t>
+  </si>
+  <si>
+    <t>69,69,69</t>
+  </si>
+  <si>
+    <t>14,17,19</t>
+  </si>
+  <si>
+    <t>19,23,25</t>
+  </si>
+  <si>
+    <t>27,31,31</t>
+  </si>
+  <si>
+    <t>32,33,37</t>
+  </si>
+  <si>
+    <t>45,45,48</t>
+  </si>
+  <si>
+    <t>48,49,49</t>
+  </si>
+  <si>
+    <t>53,75,79</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (x-µ)/σ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am using 2 decimal places since the max data is 65, therefore I am divding by 100 </t>
+  </si>
+  <si>
+    <t>sepalwidth</t>
+  </si>
+  <si>
+    <t>Decimal</t>
+  </si>
+  <si>
+    <t>Min Max 0-10</t>
+  </si>
+  <si>
+    <t>Z score</t>
+  </si>
+  <si>
+    <t>decimal scaling to 2 decimal places would keep the range the smallest out of the three normaization methods, however the parameter of 10 must be preserved</t>
+  </si>
+  <si>
+    <t>Z score normalization attemps to reduce the effect of outliers on the transformed data, but the scale is changed so intervals are not exactly the same as the original data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">with the paramters of 0 to 1 for the new values are distributed similarly to the unnormailzed data. one issue that didn’t occur in this dataset, but can with others, is if there is an outlier it will stay an outlyer and skew the data. </t>
   </si>
 </sst>
 </file>
@@ -1458,8 +1527,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -1587,7 +1656,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1603,6 +1672,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1767,7 +1842,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1881,8 +1956,28 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1893,21 +1988,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3849,7 +3938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -3891,7 +3980,7 @@
         <v>382</v>
       </c>
       <c r="C9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -4952,10 +5041,10 @@
       <c r="B68" s="25"/>
       <c r="C68" s="25"/>
       <c r="D68" s="25"/>
-      <c r="E68" s="61" t="s">
+      <c r="E68" s="71" t="s">
         <v>366</v>
       </c>
-      <c r="F68" s="61"/>
+      <c r="F68" s="71"/>
       <c r="G68" s="48">
         <f>-G67</f>
         <v>1.5566567074628228</v>
@@ -4982,13 +5071,13 @@
       <c r="D71" s="25"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="62" t="s">
+      <c r="A72" s="72" t="s">
         <v>367</v>
       </c>
-      <c r="B72" s="61"/>
-      <c r="C72" s="61"/>
-      <c r="D72" s="61"/>
-      <c r="E72" s="61"/>
+      <c r="B72" s="71"/>
+      <c r="C72" s="71"/>
+      <c r="D72" s="71"/>
+      <c r="E72" s="71"/>
       <c r="F72" s="48">
         <f>D58/G68</f>
         <v>1.8772646222418671E-2</v>
@@ -7215,63 +7304,63 @@
       <c r="B50" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="C50" s="63" t="s">
+      <c r="C50" s="74" t="s">
         <v>174</v>
       </c>
-      <c r="D50" s="63"/>
-      <c r="E50" s="63"/>
-      <c r="F50" s="63"/>
-      <c r="G50" s="63"/>
+      <c r="D50" s="74"/>
+      <c r="E50" s="74"/>
+      <c r="F50" s="74"/>
+      <c r="G50" s="74"/>
       <c r="H50" s="26" t="s">
         <v>175</v>
       </c>
       <c r="I50" s="26"/>
-      <c r="J50" s="63" t="s">
+      <c r="J50" s="74" t="s">
         <v>176</v>
       </c>
-      <c r="K50" s="63"/>
+      <c r="K50" s="74"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B51" s="24">
         <v>4</v>
       </c>
-      <c r="C51" s="64"/>
-      <c r="D51" s="64"/>
-      <c r="E51" s="64"/>
-      <c r="F51" s="64"/>
-      <c r="G51" s="64"/>
-      <c r="H51" s="65"/>
-      <c r="I51" s="65"/>
-      <c r="J51" s="65"/>
-      <c r="K51" s="65"/>
+      <c r="C51" s="73"/>
+      <c r="D51" s="73"/>
+      <c r="E51" s="73"/>
+      <c r="F51" s="73"/>
+      <c r="G51" s="73"/>
+      <c r="H51" s="75"/>
+      <c r="I51" s="75"/>
+      <c r="J51" s="75"/>
+      <c r="K51" s="75"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B52" s="24">
         <v>5</v>
       </c>
-      <c r="C52" s="64"/>
-      <c r="D52" s="64"/>
-      <c r="E52" s="64"/>
-      <c r="F52" s="64"/>
-      <c r="G52" s="64"/>
-      <c r="H52" s="65"/>
-      <c r="I52" s="65"/>
-      <c r="J52" s="65"/>
-      <c r="K52" s="65"/>
+      <c r="C52" s="73"/>
+      <c r="D52" s="73"/>
+      <c r="E52" s="73"/>
+      <c r="F52" s="73"/>
+      <c r="G52" s="73"/>
+      <c r="H52" s="75"/>
+      <c r="I52" s="75"/>
+      <c r="J52" s="75"/>
+      <c r="K52" s="75"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B53" s="24">
         <v>6</v>
       </c>
-      <c r="C53" s="64"/>
-      <c r="D53" s="64"/>
-      <c r="E53" s="64"/>
-      <c r="F53" s="64"/>
-      <c r="G53" s="64"/>
-      <c r="H53" s="65"/>
-      <c r="I53" s="65"/>
-      <c r="J53" s="65"/>
-      <c r="K53" s="65"/>
+      <c r="C53" s="73"/>
+      <c r="D53" s="73"/>
+      <c r="E53" s="73"/>
+      <c r="F53" s="73"/>
+      <c r="G53" s="73"/>
+      <c r="H53" s="75"/>
+      <c r="I53" s="75"/>
+      <c r="J53" s="75"/>
+      <c r="K53" s="75"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
@@ -7300,61 +7389,61 @@
       <c r="B61" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="C61" s="63" t="s">
+      <c r="C61" s="74" t="s">
         <v>182</v>
       </c>
-      <c r="D61" s="63"/>
-      <c r="E61" s="63"/>
-      <c r="F61" s="63"/>
-      <c r="G61" s="63"/>
-      <c r="H61" s="63"/>
-      <c r="I61" s="63"/>
-      <c r="J61" s="63" t="s">
+      <c r="D61" s="74"/>
+      <c r="E61" s="74"/>
+      <c r="F61" s="74"/>
+      <c r="G61" s="74"/>
+      <c r="H61" s="74"/>
+      <c r="I61" s="74"/>
+      <c r="J61" s="74" t="s">
         <v>183</v>
       </c>
-      <c r="K61" s="63"/>
+      <c r="K61" s="74"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B62" s="24">
         <v>6</v>
       </c>
-      <c r="C62" s="64"/>
-      <c r="D62" s="64"/>
-      <c r="E62" s="64"/>
-      <c r="F62" s="64"/>
-      <c r="G62" s="64"/>
-      <c r="H62" s="64"/>
-      <c r="I62" s="64"/>
-      <c r="J62" s="64"/>
-      <c r="K62" s="64"/>
+      <c r="C62" s="73"/>
+      <c r="D62" s="73"/>
+      <c r="E62" s="73"/>
+      <c r="F62" s="73"/>
+      <c r="G62" s="73"/>
+      <c r="H62" s="73"/>
+      <c r="I62" s="73"/>
+      <c r="J62" s="73"/>
+      <c r="K62" s="73"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B63" s="24">
         <v>5</v>
       </c>
-      <c r="C63" s="64"/>
-      <c r="D63" s="64"/>
-      <c r="E63" s="64"/>
-      <c r="F63" s="64"/>
-      <c r="G63" s="64"/>
-      <c r="H63" s="64"/>
-      <c r="I63" s="64"/>
-      <c r="J63" s="64"/>
-      <c r="K63" s="64"/>
+      <c r="C63" s="73"/>
+      <c r="D63" s="73"/>
+      <c r="E63" s="73"/>
+      <c r="F63" s="73"/>
+      <c r="G63" s="73"/>
+      <c r="H63" s="73"/>
+      <c r="I63" s="73"/>
+      <c r="J63" s="73"/>
+      <c r="K63" s="73"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B64" s="24">
         <v>4</v>
       </c>
-      <c r="C64" s="64"/>
-      <c r="D64" s="64"/>
-      <c r="E64" s="64"/>
-      <c r="F64" s="64"/>
-      <c r="G64" s="64"/>
-      <c r="H64" s="64"/>
-      <c r="I64" s="64"/>
-      <c r="J64" s="64"/>
-      <c r="K64" s="64"/>
+      <c r="C64" s="73"/>
+      <c r="D64" s="73"/>
+      <c r="E64" s="73"/>
+      <c r="F64" s="73"/>
+      <c r="G64" s="73"/>
+      <c r="H64" s="73"/>
+      <c r="I64" s="73"/>
+      <c r="J64" s="73"/>
+      <c r="K64" s="73"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
@@ -7392,19 +7481,19 @@
       <c r="C74" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="D74" s="63" t="s">
+      <c r="D74" s="74" t="s">
         <v>191</v>
       </c>
-      <c r="E74" s="63"/>
-      <c r="F74" s="63"/>
-      <c r="G74" s="63"/>
-      <c r="H74" s="63"/>
-      <c r="I74" s="63"/>
-      <c r="J74" s="63" t="s">
+      <c r="E74" s="74"/>
+      <c r="F74" s="74"/>
+      <c r="G74" s="74"/>
+      <c r="H74" s="74"/>
+      <c r="I74" s="74"/>
+      <c r="J74" s="74" t="s">
         <v>192</v>
       </c>
-      <c r="K74" s="63"/>
-      <c r="L74" s="63"/>
+      <c r="K74" s="74"/>
+      <c r="L74" s="74"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B75" s="29" t="s">
@@ -7413,15 +7502,15 @@
       <c r="C75" s="24">
         <v>1</v>
       </c>
-      <c r="D75" s="64"/>
-      <c r="E75" s="64"/>
-      <c r="F75" s="64"/>
-      <c r="G75" s="64"/>
-      <c r="H75" s="64"/>
-      <c r="I75" s="64"/>
-      <c r="J75" s="64"/>
-      <c r="K75" s="64"/>
-      <c r="L75" s="64"/>
+      <c r="D75" s="73"/>
+      <c r="E75" s="73"/>
+      <c r="F75" s="73"/>
+      <c r="G75" s="73"/>
+      <c r="H75" s="73"/>
+      <c r="I75" s="73"/>
+      <c r="J75" s="73"/>
+      <c r="K75" s="73"/>
+      <c r="L75" s="73"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B76" s="29" t="s">
@@ -7430,15 +7519,15 @@
       <c r="C76" s="24">
         <v>1</v>
       </c>
-      <c r="D76" s="64"/>
-      <c r="E76" s="64"/>
-      <c r="F76" s="64"/>
-      <c r="G76" s="64"/>
-      <c r="H76" s="64"/>
-      <c r="I76" s="64"/>
-      <c r="J76" s="64"/>
-      <c r="K76" s="64"/>
-      <c r="L76" s="64"/>
+      <c r="D76" s="73"/>
+      <c r="E76" s="73"/>
+      <c r="F76" s="73"/>
+      <c r="G76" s="73"/>
+      <c r="H76" s="73"/>
+      <c r="I76" s="73"/>
+      <c r="J76" s="73"/>
+      <c r="K76" s="73"/>
+      <c r="L76" s="73"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B77" s="29" t="s">
@@ -7447,15 +7536,15 @@
       <c r="C77" s="24">
         <v>0</v>
       </c>
-      <c r="D77" s="64"/>
-      <c r="E77" s="64"/>
-      <c r="F77" s="64"/>
-      <c r="G77" s="64"/>
-      <c r="H77" s="64"/>
-      <c r="I77" s="64"/>
-      <c r="J77" s="64"/>
-      <c r="K77" s="64"/>
-      <c r="L77" s="64"/>
+      <c r="D77" s="73"/>
+      <c r="E77" s="73"/>
+      <c r="F77" s="73"/>
+      <c r="G77" s="73"/>
+      <c r="H77" s="73"/>
+      <c r="I77" s="73"/>
+      <c r="J77" s="73"/>
+      <c r="K77" s="73"/>
+      <c r="L77" s="73"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B78" s="29" t="s">
@@ -7464,15 +7553,15 @@
       <c r="C78" s="24">
         <v>0.19214789423111006</v>
       </c>
-      <c r="D78" s="64"/>
-      <c r="E78" s="64"/>
-      <c r="F78" s="64"/>
-      <c r="G78" s="64"/>
-      <c r="H78" s="64"/>
-      <c r="I78" s="64"/>
-      <c r="J78" s="64"/>
-      <c r="K78" s="64"/>
-      <c r="L78" s="64"/>
+      <c r="D78" s="73"/>
+      <c r="E78" s="73"/>
+      <c r="F78" s="73"/>
+      <c r="G78" s="73"/>
+      <c r="H78" s="73"/>
+      <c r="I78" s="73"/>
+      <c r="J78" s="73"/>
+      <c r="K78" s="73"/>
+      <c r="L78" s="73"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B79" s="29" t="s">
@@ -7481,15 +7570,15 @@
       <c r="C79" s="24">
         <v>-0.30588787655775207</v>
       </c>
-      <c r="D79" s="64"/>
-      <c r="E79" s="64"/>
-      <c r="F79" s="64"/>
-      <c r="G79" s="64"/>
-      <c r="H79" s="64"/>
-      <c r="I79" s="64"/>
-      <c r="J79" s="64"/>
-      <c r="K79" s="64"/>
-      <c r="L79" s="64"/>
+      <c r="D79" s="73"/>
+      <c r="E79" s="73"/>
+      <c r="F79" s="73"/>
+      <c r="G79" s="73"/>
+      <c r="H79" s="73"/>
+      <c r="I79" s="73"/>
+      <c r="J79" s="73"/>
+      <c r="K79" s="73"/>
+      <c r="L79" s="73"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B80" s="29" t="s">
@@ -7498,15 +7587,15 @@
       <c r="C80" s="24">
         <v>0.4</v>
       </c>
-      <c r="D80" s="64"/>
-      <c r="E80" s="64"/>
-      <c r="F80" s="64"/>
-      <c r="G80" s="64"/>
-      <c r="H80" s="64"/>
-      <c r="I80" s="64"/>
-      <c r="J80" s="64"/>
-      <c r="K80" s="64"/>
-      <c r="L80" s="64"/>
+      <c r="D80" s="73"/>
+      <c r="E80" s="73"/>
+      <c r="F80" s="73"/>
+      <c r="G80" s="73"/>
+      <c r="H80" s="73"/>
+      <c r="I80" s="73"/>
+      <c r="J80" s="73"/>
+      <c r="K80" s="73"/>
+      <c r="L80" s="73"/>
     </row>
     <row r="81" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B81" s="29" t="s">
@@ -7515,15 +7604,15 @@
       <c r="C81" s="24">
         <v>0.1</v>
       </c>
-      <c r="D81" s="64"/>
-      <c r="E81" s="64"/>
-      <c r="F81" s="64"/>
-      <c r="G81" s="64"/>
-      <c r="H81" s="64"/>
-      <c r="I81" s="64"/>
-      <c r="J81" s="64"/>
-      <c r="K81" s="64"/>
-      <c r="L81" s="64"/>
+      <c r="D81" s="73"/>
+      <c r="E81" s="73"/>
+      <c r="F81" s="73"/>
+      <c r="G81" s="73"/>
+      <c r="H81" s="73"/>
+      <c r="I81" s="73"/>
+      <c r="J81" s="73"/>
+      <c r="K81" s="73"/>
+      <c r="L81" s="73"/>
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B82" s="29" t="s">
@@ -7532,15 +7621,15 @@
       <c r="C82" s="24">
         <v>-0.50785210576888995</v>
       </c>
-      <c r="D82" s="64"/>
-      <c r="E82" s="64"/>
-      <c r="F82" s="64"/>
-      <c r="G82" s="64"/>
-      <c r="H82" s="64"/>
-      <c r="I82" s="64"/>
-      <c r="J82" s="64"/>
-      <c r="K82" s="64"/>
-      <c r="L82" s="64"/>
+      <c r="D82" s="73"/>
+      <c r="E82" s="73"/>
+      <c r="F82" s="73"/>
+      <c r="G82" s="73"/>
+      <c r="H82" s="73"/>
+      <c r="I82" s="73"/>
+      <c r="J82" s="73"/>
+      <c r="K82" s="73"/>
+      <c r="L82" s="73"/>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B83" s="29" t="s">
@@ -7549,15 +7638,15 @@
       <c r="C83" s="24">
         <v>0.19411212344224793</v>
       </c>
-      <c r="D83" s="64"/>
-      <c r="E83" s="64"/>
-      <c r="F83" s="64"/>
-      <c r="G83" s="64"/>
-      <c r="H83" s="64"/>
-      <c r="I83" s="64"/>
-      <c r="J83" s="64"/>
-      <c r="K83" s="64"/>
-      <c r="L83" s="64"/>
+      <c r="D83" s="73"/>
+      <c r="E83" s="73"/>
+      <c r="F83" s="73"/>
+      <c r="G83" s="73"/>
+      <c r="H83" s="73"/>
+      <c r="I83" s="73"/>
+      <c r="J83" s="73"/>
+      <c r="K83" s="73"/>
+      <c r="L83" s="73"/>
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B84" s="29" t="s">
@@ -7566,15 +7655,15 @@
       <c r="C84" s="24">
         <v>-0.26082884634154524</v>
       </c>
-      <c r="D84" s="64"/>
-      <c r="E84" s="64"/>
-      <c r="F84" s="64"/>
-      <c r="G84" s="64"/>
-      <c r="H84" s="64"/>
-      <c r="I84" s="64"/>
-      <c r="J84" s="64"/>
-      <c r="K84" s="64"/>
-      <c r="L84" s="64"/>
+      <c r="D84" s="73"/>
+      <c r="E84" s="73"/>
+      <c r="F84" s="73"/>
+      <c r="G84" s="73"/>
+      <c r="H84" s="73"/>
+      <c r="I84" s="73"/>
+      <c r="J84" s="73"/>
+      <c r="K84" s="73"/>
+      <c r="L84" s="73"/>
     </row>
     <row r="85" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B85" s="29" t="s">
@@ -7583,15 +7672,15 @@
       <c r="C85" s="24">
         <v>-0.13802506750700472</v>
       </c>
-      <c r="D85" s="64"/>
-      <c r="E85" s="64"/>
-      <c r="F85" s="64"/>
-      <c r="G85" s="64"/>
-      <c r="H85" s="64"/>
-      <c r="I85" s="64"/>
-      <c r="J85" s="64"/>
-      <c r="K85" s="64"/>
-      <c r="L85" s="64"/>
+      <c r="D85" s="73"/>
+      <c r="E85" s="73"/>
+      <c r="F85" s="73"/>
+      <c r="G85" s="73"/>
+      <c r="H85" s="73"/>
+      <c r="I85" s="73"/>
+      <c r="J85" s="73"/>
+      <c r="K85" s="73"/>
+      <c r="L85" s="73"/>
     </row>
     <row r="86" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B86" s="30" t="s">
@@ -7600,15 +7689,15 @@
       <c r="C86" s="24">
         <v>-0.40785210576888997</v>
       </c>
-      <c r="D86" s="64"/>
-      <c r="E86" s="64"/>
-      <c r="F86" s="64"/>
-      <c r="G86" s="64"/>
-      <c r="H86" s="64"/>
-      <c r="I86" s="64"/>
-      <c r="J86" s="64"/>
-      <c r="K86" s="64"/>
-      <c r="L86" s="64"/>
+      <c r="D86" s="73"/>
+      <c r="E86" s="73"/>
+      <c r="F86" s="73"/>
+      <c r="G86" s="73"/>
+      <c r="H86" s="73"/>
+      <c r="I86" s="73"/>
+      <c r="J86" s="73"/>
+      <c r="K86" s="73"/>
+      <c r="L86" s="73"/>
     </row>
     <row r="87" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B87" s="30" t="s">
@@ -7617,15 +7706,15 @@
       <c r="C87" s="24">
         <v>0.19411212344224793</v>
       </c>
-      <c r="D87" s="64"/>
-      <c r="E87" s="64"/>
-      <c r="F87" s="64"/>
-      <c r="G87" s="64"/>
-      <c r="H87" s="64"/>
-      <c r="I87" s="64"/>
-      <c r="J87" s="64"/>
-      <c r="K87" s="64"/>
-      <c r="L87" s="64"/>
+      <c r="D87" s="73"/>
+      <c r="E87" s="73"/>
+      <c r="F87" s="73"/>
+      <c r="G87" s="73"/>
+      <c r="H87" s="73"/>
+      <c r="I87" s="73"/>
+      <c r="J87" s="73"/>
+      <c r="K87" s="73"/>
+      <c r="L87" s="73"/>
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B88" s="30" t="s">
@@ -7634,52 +7723,18 @@
       <c r="C88" s="24">
         <v>0.21805217039291008</v>
       </c>
-      <c r="D88" s="64"/>
-      <c r="E88" s="64"/>
-      <c r="F88" s="64"/>
-      <c r="G88" s="64"/>
-      <c r="H88" s="64"/>
-      <c r="I88" s="64"/>
-      <c r="J88" s="64"/>
-      <c r="K88" s="64"/>
-      <c r="L88" s="64"/>
+      <c r="D88" s="73"/>
+      <c r="E88" s="73"/>
+      <c r="F88" s="73"/>
+      <c r="G88" s="73"/>
+      <c r="H88" s="73"/>
+      <c r="I88" s="73"/>
+      <c r="J88" s="73"/>
+      <c r="K88" s="73"/>
+      <c r="L88" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="D87:I87"/>
-    <mergeCell ref="J87:L87"/>
-    <mergeCell ref="D88:I88"/>
-    <mergeCell ref="J88:L88"/>
-    <mergeCell ref="D84:I84"/>
-    <mergeCell ref="J84:L84"/>
-    <mergeCell ref="D85:I85"/>
-    <mergeCell ref="J85:L85"/>
-    <mergeCell ref="D86:I86"/>
-    <mergeCell ref="J86:L86"/>
-    <mergeCell ref="D81:I81"/>
-    <mergeCell ref="J81:L81"/>
-    <mergeCell ref="D82:I82"/>
-    <mergeCell ref="J82:L82"/>
-    <mergeCell ref="D83:I83"/>
-    <mergeCell ref="J83:L83"/>
-    <mergeCell ref="D78:I78"/>
-    <mergeCell ref="J78:L78"/>
-    <mergeCell ref="D79:I79"/>
-    <mergeCell ref="J79:L79"/>
-    <mergeCell ref="D80:I80"/>
-    <mergeCell ref="J80:L80"/>
-    <mergeCell ref="D75:I75"/>
-    <mergeCell ref="J75:L75"/>
-    <mergeCell ref="D76:I76"/>
-    <mergeCell ref="J76:L76"/>
-    <mergeCell ref="D77:I77"/>
-    <mergeCell ref="J77:L77"/>
-    <mergeCell ref="C63:I63"/>
-    <mergeCell ref="J63:K63"/>
-    <mergeCell ref="C64:I64"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="D74:I74"/>
-    <mergeCell ref="J74:L74"/>
     <mergeCell ref="C50:G50"/>
     <mergeCell ref="J50:K50"/>
     <mergeCell ref="C62:I62"/>
@@ -7695,6 +7750,40 @@
     <mergeCell ref="J53:K53"/>
     <mergeCell ref="C61:I61"/>
     <mergeCell ref="J61:K61"/>
+    <mergeCell ref="C63:I63"/>
+    <mergeCell ref="J63:K63"/>
+    <mergeCell ref="C64:I64"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="D74:I74"/>
+    <mergeCell ref="J74:L74"/>
+    <mergeCell ref="D75:I75"/>
+    <mergeCell ref="J75:L75"/>
+    <mergeCell ref="D76:I76"/>
+    <mergeCell ref="J76:L76"/>
+    <mergeCell ref="D77:I77"/>
+    <mergeCell ref="J77:L77"/>
+    <mergeCell ref="D78:I78"/>
+    <mergeCell ref="J78:L78"/>
+    <mergeCell ref="D79:I79"/>
+    <mergeCell ref="J79:L79"/>
+    <mergeCell ref="D80:I80"/>
+    <mergeCell ref="J80:L80"/>
+    <mergeCell ref="D81:I81"/>
+    <mergeCell ref="J81:L81"/>
+    <mergeCell ref="D82:I82"/>
+    <mergeCell ref="J82:L82"/>
+    <mergeCell ref="D83:I83"/>
+    <mergeCell ref="J83:L83"/>
+    <mergeCell ref="D87:I87"/>
+    <mergeCell ref="J87:L87"/>
+    <mergeCell ref="D88:I88"/>
+    <mergeCell ref="J88:L88"/>
+    <mergeCell ref="D84:I84"/>
+    <mergeCell ref="J84:L84"/>
+    <mergeCell ref="D85:I85"/>
+    <mergeCell ref="J85:L85"/>
+    <mergeCell ref="D86:I86"/>
+    <mergeCell ref="J86:L86"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7767,7 +7856,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7919,10 +8008,10 @@
         <v>1</v>
       </c>
       <c r="K7" s="24"/>
-      <c r="L7" s="59" t="s">
+      <c r="L7" s="68" t="s">
         <v>397</v>
       </c>
-      <c r="M7" s="59"/>
+      <c r="M7" s="68"/>
     </row>
     <row r="8" spans="1:13" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -8133,10 +8222,10 @@
       <c r="K16" s="24" t="s">
         <v>410</v>
       </c>
-      <c r="L16" s="59" t="s">
+      <c r="L16" s="68" t="s">
         <v>411</v>
       </c>
-      <c r="M16" s="59"/>
+      <c r="M16" s="68"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -8367,15 +8456,15 @@
       <c r="C4">
         <v>53</v>
       </c>
-      <c r="D4" s="67">
+      <c r="D4" s="61">
         <f>C4/200</f>
         <v>0.26500000000000001</v>
       </c>
-      <c r="E4" s="67">
+      <c r="E4" s="61">
         <f>SUM(D4)</f>
         <v>0.26500000000000001</v>
       </c>
-      <c r="G4" s="68"/>
+      <c r="G4" s="62"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -8384,11 +8473,11 @@
       <c r="C5">
         <v>37</v>
       </c>
-      <c r="D5" s="67">
+      <c r="D5" s="61">
         <f t="shared" ref="D5:D10" si="0">C5/200</f>
         <v>0.185</v>
       </c>
-      <c r="E5" s="67">
+      <c r="E5" s="61">
         <f>SUM(D4:D5)</f>
         <v>0.45</v>
       </c>
@@ -8400,11 +8489,11 @@
       <c r="C6">
         <v>65</v>
       </c>
-      <c r="D6" s="67">
+      <c r="D6" s="61">
         <f t="shared" si="0"/>
         <v>0.32500000000000001</v>
       </c>
-      <c r="E6" s="67">
+      <c r="E6" s="61">
         <f>SUM(D4:D6)</f>
         <v>0.77500000000000002</v>
       </c>
@@ -8416,11 +8505,11 @@
       <c r="C7">
         <v>18</v>
       </c>
-      <c r="D7" s="67">
+      <c r="D7" s="61">
         <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
-      <c r="E7" s="67">
+      <c r="E7" s="61">
         <f>SUM(D4:D7)</f>
         <v>0.86499999999999999</v>
       </c>
@@ -8432,11 +8521,11 @@
       <c r="C8">
         <v>12</v>
       </c>
-      <c r="D8" s="67">
+      <c r="D8" s="61">
         <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
-      <c r="E8" s="67">
+      <c r="E8" s="61">
         <f>SUM(D4:D8)</f>
         <v>0.92500000000000004</v>
       </c>
@@ -8448,11 +8537,11 @@
       <c r="C9">
         <v>13</v>
       </c>
-      <c r="D9" s="67">
+      <c r="D9" s="61">
         <f t="shared" si="0"/>
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E9" s="67">
+      <c r="E9" s="61">
         <f>SUM(D4:D9)</f>
         <v>0.99</v>
       </c>
@@ -8464,11 +8553,11 @@
       <c r="C10">
         <v>2</v>
       </c>
-      <c r="D10" s="67">
+      <c r="D10" s="61">
         <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="E10" s="67">
+      <c r="E10" s="61">
         <f>SUM(D4:D10)</f>
         <v>1</v>
       </c>
@@ -8483,11 +8572,11 @@
       <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="66" t="s">
+      <c r="B13" s="69" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
       <c r="E13">
         <v>5</v>
       </c>
@@ -8496,11 +8585,11 @@
       <c r="A14" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="66" t="s">
+      <c r="B14" s="69" t="s">
         <v>73</v>
       </c>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
       <c r="E14">
         <v>200</v>
       </c>
@@ -8509,11 +8598,11 @@
       <c r="A15" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="69" t="s">
         <v>412</v>
       </c>
-      <c r="C15" s="66"/>
-      <c r="D15" s="66"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
       <c r="E15" s="57">
         <v>0.09</v>
       </c>
@@ -8522,11 +8611,11 @@
       <c r="A16" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="69" t="s">
         <v>413</v>
       </c>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
       <c r="E16">
         <v>0.86499999999999999</v>
       </c>
@@ -8549,7 +8638,7 @@
       <c r="B18" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="67">
+      <c r="E18" s="61">
         <f xml:space="preserve"> 10 + (((200/2) - 0.45)/65)*5</f>
         <v>17.657692307692308</v>
       </c>
@@ -8603,7 +8692,7 @@
       <c r="C28" t="s">
         <v>85</v>
       </c>
-      <c r="D28" s="67">
+      <c r="D28" s="61">
         <f>E18</f>
         <v>17.657692307692308</v>
       </c>
@@ -8750,7 +8839,7 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <f t="shared" ref="D14:D16" si="0">(B14-C14)^2</f>
+        <f>(B14-C14)^2</f>
         <v>9</v>
       </c>
       <c r="F14">
@@ -8772,7 +8861,7 @@
         <v>17</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f>(B15-C15)^2</f>
         <v>9</v>
       </c>
       <c r="F15">
@@ -8794,7 +8883,7 @@
         <v>9</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f>(B16-C16)^2</f>
         <v>4</v>
       </c>
       <c r="F16">
@@ -8828,7 +8917,7 @@
       <c r="C18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="69">
+      <c r="D18" s="63">
         <f>SQRT(D17)</f>
         <v>7.6157731058639087</v>
       </c>
@@ -8898,7 +8987,7 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <f t="shared" ref="D25:D28" si="1">ABS(B25-C25)</f>
+        <f>ABS(B25-C25)</f>
         <v>3</v>
       </c>
       <c r="F25">
@@ -8920,7 +9009,7 @@
         <v>17</v>
       </c>
       <c r="D26">
-        <f t="shared" si="1"/>
+        <f>ABS(B26-C26)</f>
         <v>3</v>
       </c>
       <c r="F26">
@@ -8942,7 +9031,7 @@
         <v>9</v>
       </c>
       <c r="D27">
-        <f t="shared" si="1"/>
+        <f>ABS(B27-C27)</f>
         <v>2</v>
       </c>
       <c r="F27">
@@ -9033,7 +9122,7 @@
         <v>0</v>
       </c>
       <c r="D35">
-        <f t="shared" ref="D35:D39" si="2">ABS(B35-C35)^3</f>
+        <f>ABS(B35-C35)^3</f>
         <v>27</v>
       </c>
       <c r="F35">
@@ -9055,7 +9144,7 @@
         <v>17</v>
       </c>
       <c r="D36">
-        <f t="shared" si="2"/>
+        <f>ABS(B36-C36)^3</f>
         <v>27</v>
       </c>
       <c r="F36">
@@ -9077,7 +9166,7 @@
         <v>9</v>
       </c>
       <c r="D37">
-        <f t="shared" si="2"/>
+        <f>ABS(B37-C37)^3</f>
         <v>8</v>
       </c>
       <c r="F37">
@@ -9111,7 +9200,7 @@
       <c r="C39" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D39" s="69">
+      <c r="D39" s="63">
         <f>(D38)^(1/3)</f>
         <v>6.526518879343751</v>
       </c>
@@ -9159,7 +9248,7 @@
         <v>0</v>
       </c>
       <c r="D45">
-        <f t="shared" ref="D45:D47" si="3">ABS(B45-C45)</f>
+        <f>ABS(B45-C45)</f>
         <v>3</v>
       </c>
     </row>
@@ -9171,7 +9260,7 @@
         <v>17</v>
       </c>
       <c r="D46">
-        <f t="shared" si="3"/>
+        <f>ABS(B46-C46)</f>
         <v>3</v>
       </c>
     </row>
@@ -9183,7 +9272,7 @@
         <v>9</v>
       </c>
       <c r="D47">
-        <f t="shared" si="3"/>
+        <f>ABS(B47-C47)</f>
         <v>2</v>
       </c>
     </row>
@@ -9207,12 +9296,12 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="3.85546875" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.140625" customWidth="1"/>
     <col min="6" max="6" width="3.85546875" customWidth="1"/>
     <col min="7" max="7" width="6.5703125" customWidth="1"/>
@@ -9226,17 +9315,17 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="64">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="64">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="64">
         <v>19</v>
       </c>
       <c r="C4" t="s">
@@ -9269,29 +9358,85 @@
       <c r="C7" t="s">
         <v>21</v>
       </c>
+      <c r="D7" t="s">
+        <v>424</v>
+      </c>
+      <c r="H7">
+        <f>SUM(A2:A4)</f>
+        <v>50</v>
+      </c>
+      <c r="I7" s="65">
+        <f>H7/3</f>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>416</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="64">
         <v>27</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
       </c>
+      <c r="D8" t="s">
+        <v>425</v>
+      </c>
+      <c r="H8">
+        <f>SUM(A5:A7)</f>
+        <v>67</v>
+      </c>
+      <c r="I8" s="65">
+        <f t="shared" ref="I8:I14" si="0">H8/3</f>
+        <v>22.333333333333332</v>
+      </c>
+      <c r="J8" s="60" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="64">
         <v>31</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
       </c>
+      <c r="D9" t="s">
+        <v>426</v>
+      </c>
+      <c r="H9">
+        <f>SUM(A8:A10)</f>
+        <v>89</v>
+      </c>
+      <c r="I9" s="65">
+        <f t="shared" si="0"/>
+        <v>29.666666666666668</v>
+      </c>
+      <c r="J9" s="60" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="64">
         <v>31</v>
       </c>
       <c r="C10" t="s">
         <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>427</v>
+      </c>
+      <c r="H10">
+        <f>SUM(A11:A13)</f>
+        <v>102</v>
+      </c>
+      <c r="I10" s="65">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="J10" s="60" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -9301,6 +9446,20 @@
       <c r="C11" t="s">
         <v>25</v>
       </c>
+      <c r="D11" t="s">
+        <v>420</v>
+      </c>
+      <c r="H11">
+        <f>SUM(A14:A16)</f>
+        <v>111</v>
+      </c>
+      <c r="I11" s="65">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="J11" s="60" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -9309,6 +9468,20 @@
       <c r="C12" t="s">
         <v>26</v>
       </c>
+      <c r="D12" t="s">
+        <v>428</v>
+      </c>
+      <c r="H12">
+        <f>SUM(A17:A19)</f>
+        <v>138</v>
+      </c>
+      <c r="I12" s="65">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="J12" s="60" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -9317,22 +9490,50 @@
       <c r="C13" t="s">
         <v>27</v>
       </c>
+      <c r="D13" t="s">
+        <v>429</v>
+      </c>
+      <c r="H13">
+        <f>SUM(A20:A22)</f>
+        <v>146</v>
+      </c>
+      <c r="I13" s="65">
+        <f t="shared" si="0"/>
+        <v>48.666666666666664</v>
+      </c>
+      <c r="J13" s="60" t="s">
+        <v>422</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="64">
         <v>37</v>
       </c>
       <c r="C14" t="s">
         <v>28</v>
       </c>
+      <c r="D14" t="s">
+        <v>430</v>
+      </c>
+      <c r="H14">
+        <f>SUM(A23:A25)</f>
+        <v>207</v>
+      </c>
+      <c r="I14" s="65">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="J14" s="60" t="s">
+        <v>423</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="64">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="64">
         <v>37</v>
       </c>
     </row>
@@ -9352,17 +9553,17 @@
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="64">
         <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="64">
         <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="64">
         <v>49</v>
       </c>
     </row>
@@ -9389,29 +9590,61 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:R152"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="4.140625" customWidth="1"/>
     <col min="4" max="4" width="4" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M1" s="66"/>
+      <c r="O1" s="4">
+        <f>MIN(M3:M152)</f>
+        <v>2</v>
+      </c>
+      <c r="P1" s="4">
+        <f>MAX(M3:M152)</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Q1" s="4">
+        <f>_xlfn.STDEV.S(M3:M152)</f>
+        <v>0.4335943113621879</v>
+      </c>
+      <c r="R1" s="4">
+        <f>(SUM(M3:M152)/COUNT(M3:M152))</f>
+        <v>3.053999999999998</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M2" s="66" t="s">
+        <v>433</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>14</v>
       </c>
@@ -9421,76 +9654,248 @@
       <c r="D3" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M3" s="66">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <f>M3/10</f>
+        <v>0.2</v>
+      </c>
+      <c r="O3" s="58">
+        <f>((M3-2)/(4.4-2))*(1-0)+0</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="58">
+        <f>(M3-0.433594)/3.054</f>
+        <v>0.51290307793058287</v>
+      </c>
+      <c r="Q3" s="58">
+        <f>P152-P3</f>
+        <v>0.78585461689587455</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>17</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M4" s="66">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:N67" si="0">M4/10</f>
+        <v>0.22000000000000003</v>
+      </c>
+      <c r="O4" s="58">
+        <f t="shared" ref="O4:O67" si="1">((M4-2)/(4.4-2))*(1-0)+0</f>
+        <v>8.3333333333333398E-2</v>
+      </c>
+      <c r="P4" s="58">
+        <f t="shared" ref="P4:P67" si="2">(M4-0.433594)/3.054</f>
+        <v>0.57839096267190582</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>19</v>
       </c>
       <c r="E5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>53</v>
+      </c>
+      <c r="M5" s="66">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>0.22000000000000003</v>
+      </c>
+      <c r="O5" s="58">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333398E-2</v>
+      </c>
+      <c r="P5" s="58">
+        <f t="shared" si="2"/>
+        <v>0.57839096267190582</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>19</v>
       </c>
       <c r="E6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>14</v>
+      </c>
+      <c r="M6" s="66">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>0.22000000000000003</v>
+      </c>
+      <c r="O6" s="58">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333398E-2</v>
+      </c>
+      <c r="P6" s="58">
+        <f t="shared" si="2"/>
+        <v>0.57839096267190582</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>23</v>
       </c>
       <c r="E7" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>80</v>
+      </c>
+      <c r="M7" s="66">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>0.22999999999999998</v>
+      </c>
+      <c r="O7" s="58">
+        <f t="shared" si="1"/>
+        <v>0.1249999999999999</v>
+      </c>
+      <c r="P7" s="58">
+        <f t="shared" si="2"/>
+        <v>0.61113490504256707</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>25</v>
       </c>
       <c r="E8" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="63">
+        <v>0</v>
+      </c>
+      <c r="M8" s="66">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>0.22999999999999998</v>
+      </c>
+      <c r="O8" s="58">
+        <f t="shared" si="1"/>
+        <v>0.1249999999999999</v>
+      </c>
+      <c r="P8" s="58">
+        <f t="shared" si="2"/>
+        <v>0.61113490504256707</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>27</v>
       </c>
       <c r="E9" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="63">
+        <v>1</v>
+      </c>
+      <c r="M9" s="66">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>0.22999999999999998</v>
+      </c>
+      <c r="O9" s="58">
+        <f t="shared" si="1"/>
+        <v>0.1249999999999999</v>
+      </c>
+      <c r="P9" s="58">
+        <f t="shared" si="2"/>
+        <v>0.61113490504256707</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>31</v>
       </c>
       <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M10" s="66">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>0.22999999999999998</v>
+      </c>
+      <c r="O10" s="58">
+        <f t="shared" si="1"/>
+        <v>0.1249999999999999</v>
+      </c>
+      <c r="P10" s="58">
+        <f t="shared" si="2"/>
+        <v>0.61113490504256707</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>31</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="4">
+        <f>((F5-F6)/(F7-F6))*(F9-F8)+F8</f>
+        <v>0.59090909090909094</v>
+      </c>
+      <c r="M11" s="66">
+        <v>2.4</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>0.24</v>
+      </c>
+      <c r="O11" s="58">
+        <f t="shared" si="1"/>
+        <v>0.1666666666666666</v>
+      </c>
+      <c r="P11" s="58">
+        <f t="shared" si="2"/>
+        <v>0.64387884741322854</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M12" s="66">
+        <v>2.4</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>0.24</v>
+      </c>
+      <c r="O12" s="58">
+        <f t="shared" si="1"/>
+        <v>0.1666666666666666</v>
+      </c>
+      <c r="P12" s="58">
+        <f t="shared" si="2"/>
+        <v>0.64387884741322854</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>33</v>
       </c>
@@ -9500,83 +9905,265 @@
       <c r="D13" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M13" s="66">
+        <v>2.4</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>0.24</v>
+      </c>
+      <c r="O13" s="58">
+        <f t="shared" si="1"/>
+        <v>0.1666666666666666</v>
+      </c>
+      <c r="P13" s="58">
+        <f t="shared" si="2"/>
+        <v>0.64387884741322854</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>37</v>
       </c>
       <c r="D14" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M14" s="66">
+        <v>2.5</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="O14" s="58">
+        <f t="shared" si="1"/>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="P14" s="58">
+        <f t="shared" si="2"/>
+        <v>0.67662278978389012</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>37</v>
       </c>
       <c r="D15" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M15" s="66">
+        <v>2.5</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="O15" s="58">
+        <f t="shared" si="1"/>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="P15" s="58">
+        <f t="shared" si="2"/>
+        <v>0.67662278978389012</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>37</v>
       </c>
       <c r="D16" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>53</v>
+      </c>
+      <c r="M16" s="66">
+        <v>2.5</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="O16" s="58">
+        <f t="shared" si="1"/>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="P16" s="58">
+        <f t="shared" si="2"/>
+        <v>0.67662278978389012</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>37</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <f>(SUM(A3:A27)/COUNT(A3:A27))</f>
+        <v>39.6</v>
+      </c>
+      <c r="M17" s="66">
+        <v>2.5</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="O17" s="58">
+        <f t="shared" si="1"/>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="P17" s="58">
+        <f t="shared" si="2"/>
+        <v>0.67662278978389012</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>45</v>
       </c>
       <c r="D18" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M18" s="66">
+        <v>2.5</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="O18" s="58">
+        <f t="shared" si="1"/>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="P18" s="58">
+        <f t="shared" si="2"/>
+        <v>0.67662278978389012</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M19" s="66">
+        <v>2.5</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="O19" s="58">
+        <f t="shared" si="1"/>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="P19" s="58">
+        <f t="shared" si="2"/>
+        <v>0.67662278978389012</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>48</v>
       </c>
       <c r="D20" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>431</v>
+      </c>
+      <c r="M20" s="66">
+        <v>2.5</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="O20" s="58">
+        <f t="shared" si="1"/>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="P20" s="58">
+        <f t="shared" si="2"/>
+        <v>0.67662278978389012</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>48</v>
       </c>
       <c r="D21" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <f>(53-39.6)/18.18</f>
+        <v>0.73707370737073696</v>
+      </c>
+      <c r="M21" s="66">
+        <v>2.5</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="O21" s="58">
+        <f t="shared" si="1"/>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="P21" s="58">
+        <f t="shared" si="2"/>
+        <v>0.67662278978389012</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>49</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <f>(53-39.6)/18.18</f>
+        <v>0.73707370737073696</v>
+      </c>
+      <c r="M22" s="66">
+        <v>2.6</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="0"/>
+        <v>0.26</v>
+      </c>
+      <c r="O22" s="58">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="P22" s="58">
+        <f t="shared" si="2"/>
+        <v>0.70936673215455159</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M23" s="66">
+        <v>2.6</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="0"/>
+        <v>0.26</v>
+      </c>
+      <c r="O23" s="58">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="P23" s="58">
+        <f t="shared" si="2"/>
+        <v>0.70936673215455159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>53</v>
       </c>
@@ -9586,77 +10173,2265 @@
       <c r="D24" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M24" s="66">
+        <v>2.6</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="0"/>
+        <v>0.26</v>
+      </c>
+      <c r="O24" s="58">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="P24" s="58">
+        <f t="shared" si="2"/>
+        <v>0.70936673215455159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>75</v>
       </c>
       <c r="D25" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M25" s="66">
+        <v>2.6</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="0"/>
+        <v>0.26</v>
+      </c>
+      <c r="O25" s="58">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="P25" s="58">
+        <f t="shared" si="2"/>
+        <v>0.70936673215455159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>79</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="4">
+        <v>0.53</v>
+      </c>
+      <c r="F26" t="s">
+        <v>432</v>
+      </c>
+      <c r="M26" s="66">
+        <v>2.6</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="0"/>
+        <v>0.26</v>
+      </c>
+      <c r="O26" s="58">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="P26" s="58">
+        <f t="shared" si="2"/>
+        <v>0.70936673215455159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>80</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M27" s="66">
+        <v>2.7</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="0"/>
+        <v>0.27</v>
+      </c>
+      <c r="O27" s="58">
+        <f t="shared" si="1"/>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="P27" s="58">
+        <f t="shared" si="2"/>
+        <v>0.74211067452521295</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>38</v>
       </c>
       <c r="D28" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M28" s="66">
+        <v>2.7</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="0"/>
+        <v>0.27</v>
+      </c>
+      <c r="O28" s="58">
+        <f t="shared" si="1"/>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="P28" s="58">
+        <f t="shared" si="2"/>
+        <v>0.74211067452521295</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M29" s="66">
+        <v>2.7</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="0"/>
+        <v>0.27</v>
+      </c>
+      <c r="O29" s="58">
+        <f t="shared" si="1"/>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="P29" s="58">
+        <f t="shared" si="2"/>
+        <v>0.74211067452521295</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M30" s="66">
+        <v>2.7</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="0"/>
+        <v>0.27</v>
+      </c>
+      <c r="O30" s="58">
+        <f t="shared" si="1"/>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="P30" s="58">
+        <f t="shared" si="2"/>
+        <v>0.74211067452521295</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M31" s="66">
+        <v>2.7</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="0"/>
+        <v>0.27</v>
+      </c>
+      <c r="O31" s="58">
+        <f t="shared" si="1"/>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="P31" s="58">
+        <f t="shared" si="2"/>
+        <v>0.74211067452521295</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="105" x14ac:dyDescent="0.25">
       <c r="D32" s="6" t="s">
         <v>41</v>
       </c>
       <c r="E32" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="59" t="s">
+        <v>437</v>
+      </c>
+      <c r="M32" s="66">
+        <v>2.7</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="0"/>
+        <v>0.27</v>
+      </c>
+      <c r="O32" s="58">
+        <f t="shared" si="1"/>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="P32" s="58">
+        <f t="shared" si="2"/>
+        <v>0.74211067452521295</v>
+      </c>
+    </row>
+    <row r="33" spans="4:16" ht="165" x14ac:dyDescent="0.25">
       <c r="D33" s="6" t="s">
         <v>41</v>
       </c>
       <c r="E33" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="67" t="s">
+        <v>439</v>
+      </c>
+      <c r="M33" s="66">
+        <v>2.7</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="0"/>
+        <v>0.27</v>
+      </c>
+      <c r="O33" s="58">
+        <f t="shared" si="1"/>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="P33" s="58">
+        <f t="shared" si="2"/>
+        <v>0.74211067452521295</v>
+      </c>
+    </row>
+    <row r="34" spans="4:16" ht="120" x14ac:dyDescent="0.25">
       <c r="D34" s="6" t="s">
         <v>41</v>
       </c>
       <c r="E34" t="s">
         <v>58</v>
       </c>
+      <c r="F34" s="59" t="s">
+        <v>438</v>
+      </c>
+      <c r="M34" s="66">
+        <v>2.7</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="0"/>
+        <v>0.27</v>
+      </c>
+      <c r="O34" s="58">
+        <f t="shared" si="1"/>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="P34" s="58">
+        <f t="shared" si="2"/>
+        <v>0.74211067452521295</v>
+      </c>
+    </row>
+    <row r="35" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="M35" s="66">
+        <v>2.7</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="0"/>
+        <v>0.27</v>
+      </c>
+      <c r="O35" s="58">
+        <f t="shared" si="1"/>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="P35" s="58">
+        <f t="shared" si="2"/>
+        <v>0.74211067452521295</v>
+      </c>
+    </row>
+    <row r="36" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="M36" s="66">
+        <v>2.8</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="0"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="O36" s="58">
+        <f t="shared" si="1"/>
+        <v>0.3333333333333332</v>
+      </c>
+      <c r="P36" s="58">
+        <f t="shared" si="2"/>
+        <v>0.77485461689587432</v>
+      </c>
+    </row>
+    <row r="37" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="M37" s="66">
+        <v>2.8</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="0"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="O37" s="58">
+        <f t="shared" si="1"/>
+        <v>0.3333333333333332</v>
+      </c>
+      <c r="P37" s="58">
+        <f t="shared" si="2"/>
+        <v>0.77485461689587432</v>
+      </c>
+    </row>
+    <row r="38" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="M38" s="66">
+        <v>2.8</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="0"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="O38" s="58">
+        <f t="shared" si="1"/>
+        <v>0.3333333333333332</v>
+      </c>
+      <c r="P38" s="58">
+        <f t="shared" si="2"/>
+        <v>0.77485461689587432</v>
+      </c>
+    </row>
+    <row r="39" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="M39" s="66">
+        <v>2.8</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="0"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="O39" s="58">
+        <f t="shared" si="1"/>
+        <v>0.3333333333333332</v>
+      </c>
+      <c r="P39" s="58">
+        <f t="shared" si="2"/>
+        <v>0.77485461689587432</v>
+      </c>
+    </row>
+    <row r="40" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="M40" s="66">
+        <v>2.8</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="0"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="O40" s="58">
+        <f t="shared" si="1"/>
+        <v>0.3333333333333332</v>
+      </c>
+      <c r="P40" s="58">
+        <f t="shared" si="2"/>
+        <v>0.77485461689587432</v>
+      </c>
+    </row>
+    <row r="41" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="M41" s="66">
+        <v>2.8</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="0"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="O41" s="58">
+        <f t="shared" si="1"/>
+        <v>0.3333333333333332</v>
+      </c>
+      <c r="P41" s="58">
+        <f t="shared" si="2"/>
+        <v>0.77485461689587432</v>
+      </c>
+    </row>
+    <row r="42" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="M42" s="66">
+        <v>2.8</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="0"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="O42" s="58">
+        <f t="shared" si="1"/>
+        <v>0.3333333333333332</v>
+      </c>
+      <c r="P42" s="58">
+        <f t="shared" si="2"/>
+        <v>0.77485461689587432</v>
+      </c>
+    </row>
+    <row r="43" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="M43" s="66">
+        <v>2.8</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="0"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="O43" s="58">
+        <f t="shared" si="1"/>
+        <v>0.3333333333333332</v>
+      </c>
+      <c r="P43" s="58">
+        <f t="shared" si="2"/>
+        <v>0.77485461689587432</v>
+      </c>
+    </row>
+    <row r="44" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="M44" s="66">
+        <v>2.8</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="0"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="O44" s="58">
+        <f t="shared" si="1"/>
+        <v>0.3333333333333332</v>
+      </c>
+      <c r="P44" s="58">
+        <f t="shared" si="2"/>
+        <v>0.77485461689587432</v>
+      </c>
+    </row>
+    <row r="45" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="M45" s="66">
+        <v>2.8</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="0"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="O45" s="58">
+        <f t="shared" si="1"/>
+        <v>0.3333333333333332</v>
+      </c>
+      <c r="P45" s="58">
+        <f t="shared" si="2"/>
+        <v>0.77485461689587432</v>
+      </c>
+    </row>
+    <row r="46" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="M46" s="66">
+        <v>2.8</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="0"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="O46" s="58">
+        <f t="shared" si="1"/>
+        <v>0.3333333333333332</v>
+      </c>
+      <c r="P46" s="58">
+        <f t="shared" si="2"/>
+        <v>0.77485461689587432</v>
+      </c>
+    </row>
+    <row r="47" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="M47" s="66">
+        <v>2.8</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="0"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="O47" s="58">
+        <f t="shared" si="1"/>
+        <v>0.3333333333333332</v>
+      </c>
+      <c r="P47" s="58">
+        <f t="shared" si="2"/>
+        <v>0.77485461689587432</v>
+      </c>
+    </row>
+    <row r="48" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="M48" s="66">
+        <v>2.8</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="0"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="O48" s="58">
+        <f t="shared" si="1"/>
+        <v>0.3333333333333332</v>
+      </c>
+      <c r="P48" s="58">
+        <f t="shared" si="2"/>
+        <v>0.77485461689587432</v>
+      </c>
+    </row>
+    <row r="49" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M49" s="66">
+        <v>2.8</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="0"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="O49" s="58">
+        <f t="shared" si="1"/>
+        <v>0.3333333333333332</v>
+      </c>
+      <c r="P49" s="58">
+        <f t="shared" si="2"/>
+        <v>0.77485461689587432</v>
+      </c>
+    </row>
+    <row r="50" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M50" s="66">
+        <v>2.9</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="0"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="O50" s="58">
+        <f t="shared" si="1"/>
+        <v>0.37499999999999989</v>
+      </c>
+      <c r="P50" s="58">
+        <f t="shared" si="2"/>
+        <v>0.80759855926653579</v>
+      </c>
+    </row>
+    <row r="51" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M51" s="66">
+        <v>2.9</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="0"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="O51" s="58">
+        <f t="shared" si="1"/>
+        <v>0.37499999999999989</v>
+      </c>
+      <c r="P51" s="58">
+        <f t="shared" si="2"/>
+        <v>0.80759855926653579</v>
+      </c>
+    </row>
+    <row r="52" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M52" s="66">
+        <v>2.9</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="0"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="O52" s="58">
+        <f t="shared" si="1"/>
+        <v>0.37499999999999989</v>
+      </c>
+      <c r="P52" s="58">
+        <f t="shared" si="2"/>
+        <v>0.80759855926653579</v>
+      </c>
+    </row>
+    <row r="53" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M53" s="66">
+        <v>2.9</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="0"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="O53" s="58">
+        <f t="shared" si="1"/>
+        <v>0.37499999999999989</v>
+      </c>
+      <c r="P53" s="58">
+        <f t="shared" si="2"/>
+        <v>0.80759855926653579</v>
+      </c>
+    </row>
+    <row r="54" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M54" s="66">
+        <v>2.9</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="0"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="O54" s="58">
+        <f t="shared" si="1"/>
+        <v>0.37499999999999989</v>
+      </c>
+      <c r="P54" s="58">
+        <f t="shared" si="2"/>
+        <v>0.80759855926653579</v>
+      </c>
+    </row>
+    <row r="55" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M55" s="66">
+        <v>2.9</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="0"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="O55" s="58">
+        <f t="shared" si="1"/>
+        <v>0.37499999999999989</v>
+      </c>
+      <c r="P55" s="58">
+        <f t="shared" si="2"/>
+        <v>0.80759855926653579</v>
+      </c>
+    </row>
+    <row r="56" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M56" s="66">
+        <v>2.9</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="0"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="O56" s="58">
+        <f t="shared" si="1"/>
+        <v>0.37499999999999989</v>
+      </c>
+      <c r="P56" s="58">
+        <f t="shared" si="2"/>
+        <v>0.80759855926653579</v>
+      </c>
+    </row>
+    <row r="57" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M57" s="66">
+        <v>2.9</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="0"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="O57" s="58">
+        <f t="shared" si="1"/>
+        <v>0.37499999999999989</v>
+      </c>
+      <c r="P57" s="58">
+        <f t="shared" si="2"/>
+        <v>0.80759855926653579</v>
+      </c>
+    </row>
+    <row r="58" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M58" s="66">
+        <v>2.9</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="0"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="O58" s="58">
+        <f t="shared" si="1"/>
+        <v>0.37499999999999989</v>
+      </c>
+      <c r="P58" s="58">
+        <f t="shared" si="2"/>
+        <v>0.80759855926653579</v>
+      </c>
+    </row>
+    <row r="59" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M59" s="66">
+        <v>2.9</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="0"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="O59" s="58">
+        <f t="shared" si="1"/>
+        <v>0.37499999999999989</v>
+      </c>
+      <c r="P59" s="58">
+        <f t="shared" si="2"/>
+        <v>0.80759855926653579</v>
+      </c>
+    </row>
+    <row r="60" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M60" s="66">
+        <v>3</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="O60" s="58">
+        <f t="shared" si="1"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P60" s="58">
+        <f t="shared" si="2"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="61" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M61" s="66">
+        <v>3</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="O61" s="58">
+        <f t="shared" si="1"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P61" s="58">
+        <f t="shared" si="2"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="62" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M62" s="66">
+        <v>3</v>
+      </c>
+      <c r="N62">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="O62" s="58">
+        <f t="shared" si="1"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P62" s="58">
+        <f t="shared" si="2"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="63" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M63" s="66">
+        <v>3</v>
+      </c>
+      <c r="N63">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="O63" s="58">
+        <f t="shared" si="1"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P63" s="58">
+        <f t="shared" si="2"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="64" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M64" s="66">
+        <v>3</v>
+      </c>
+      <c r="N64">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="O64" s="58">
+        <f t="shared" si="1"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P64" s="58">
+        <f t="shared" si="2"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="65" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M65" s="66">
+        <v>3</v>
+      </c>
+      <c r="N65">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="O65" s="58">
+        <f t="shared" si="1"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P65" s="58">
+        <f t="shared" si="2"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="66" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M66" s="66">
+        <v>3</v>
+      </c>
+      <c r="N66">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="O66" s="58">
+        <f t="shared" si="1"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P66" s="58">
+        <f t="shared" si="2"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="67" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M67" s="66">
+        <v>3</v>
+      </c>
+      <c r="N67">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="O67" s="58">
+        <f t="shared" si="1"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P67" s="58">
+        <f t="shared" si="2"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="68" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M68" s="66">
+        <v>3</v>
+      </c>
+      <c r="N68">
+        <f t="shared" ref="N68:N131" si="3">M68/10</f>
+        <v>0.3</v>
+      </c>
+      <c r="O68" s="58">
+        <f t="shared" ref="O68:O131" si="4">((M68-2)/(4.4-2))*(1-0)+0</f>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P68" s="58">
+        <f t="shared" ref="P68:P131" si="5">(M68-0.433594)/3.054</f>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="69" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M69" s="66">
+        <v>3</v>
+      </c>
+      <c r="N69">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="O69" s="58">
+        <f t="shared" si="4"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P69" s="58">
+        <f t="shared" si="5"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="70" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M70" s="66">
+        <v>3</v>
+      </c>
+      <c r="N70">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="O70" s="58">
+        <f t="shared" si="4"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P70" s="58">
+        <f t="shared" si="5"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="71" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M71" s="66">
+        <v>3</v>
+      </c>
+      <c r="N71">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="O71" s="58">
+        <f t="shared" si="4"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P71" s="58">
+        <f t="shared" si="5"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="72" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M72" s="66">
+        <v>3</v>
+      </c>
+      <c r="N72">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="O72" s="58">
+        <f t="shared" si="4"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P72" s="58">
+        <f t="shared" si="5"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="73" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M73" s="66">
+        <v>3</v>
+      </c>
+      <c r="N73">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="O73" s="58">
+        <f t="shared" si="4"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P73" s="58">
+        <f t="shared" si="5"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="74" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M74" s="66">
+        <v>3</v>
+      </c>
+      <c r="N74">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="O74" s="58">
+        <f t="shared" si="4"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P74" s="58">
+        <f t="shared" si="5"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="75" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M75" s="66">
+        <v>3</v>
+      </c>
+      <c r="N75">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="O75" s="58">
+        <f t="shared" si="4"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P75" s="58">
+        <f t="shared" si="5"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="76" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M76" s="66">
+        <v>3</v>
+      </c>
+      <c r="N76">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="O76" s="58">
+        <f t="shared" si="4"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P76" s="58">
+        <f t="shared" si="5"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="77" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M77" s="66">
+        <v>3</v>
+      </c>
+      <c r="N77">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="O77" s="58">
+        <f t="shared" si="4"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P77" s="58">
+        <f t="shared" si="5"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="78" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M78" s="66">
+        <v>3</v>
+      </c>
+      <c r="N78">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="O78" s="58">
+        <f t="shared" si="4"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P78" s="58">
+        <f t="shared" si="5"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="79" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M79" s="66">
+        <v>3</v>
+      </c>
+      <c r="N79">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="O79" s="58">
+        <f t="shared" si="4"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P79" s="58">
+        <f t="shared" si="5"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="80" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M80" s="66">
+        <v>3</v>
+      </c>
+      <c r="N80">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="O80" s="58">
+        <f t="shared" si="4"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P80" s="58">
+        <f t="shared" si="5"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="81" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M81" s="66">
+        <v>3</v>
+      </c>
+      <c r="N81">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="O81" s="58">
+        <f t="shared" si="4"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P81" s="58">
+        <f t="shared" si="5"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="82" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M82" s="66">
+        <v>3</v>
+      </c>
+      <c r="N82">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="O82" s="58">
+        <f t="shared" si="4"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P82" s="58">
+        <f t="shared" si="5"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="83" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M83" s="66">
+        <v>3</v>
+      </c>
+      <c r="N83">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="O83" s="58">
+        <f t="shared" si="4"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P83" s="58">
+        <f t="shared" si="5"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="84" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M84" s="66">
+        <v>3</v>
+      </c>
+      <c r="N84">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="O84" s="58">
+        <f t="shared" si="4"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P84" s="58">
+        <f t="shared" si="5"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="85" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M85" s="66">
+        <v>3</v>
+      </c>
+      <c r="N85">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="O85" s="58">
+        <f t="shared" si="4"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P85" s="58">
+        <f t="shared" si="5"/>
+        <v>0.84034250163719726</v>
+      </c>
+    </row>
+    <row r="86" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M86" s="66">
+        <v>3.1</v>
+      </c>
+      <c r="N86">
+        <f t="shared" si="3"/>
+        <v>0.31</v>
+      </c>
+      <c r="O86" s="58">
+        <f t="shared" si="4"/>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="P86" s="58">
+        <f t="shared" si="5"/>
+        <v>0.87308644400785873</v>
+      </c>
+    </row>
+    <row r="87" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M87" s="66">
+        <v>3.1</v>
+      </c>
+      <c r="N87">
+        <f t="shared" si="3"/>
+        <v>0.31</v>
+      </c>
+      <c r="O87" s="58">
+        <f t="shared" si="4"/>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="P87" s="58">
+        <f t="shared" si="5"/>
+        <v>0.87308644400785873</v>
+      </c>
+    </row>
+    <row r="88" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M88" s="66">
+        <v>3.1</v>
+      </c>
+      <c r="N88">
+        <f t="shared" si="3"/>
+        <v>0.31</v>
+      </c>
+      <c r="O88" s="58">
+        <f t="shared" si="4"/>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="P88" s="58">
+        <f t="shared" si="5"/>
+        <v>0.87308644400785873</v>
+      </c>
+    </row>
+    <row r="89" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M89" s="66">
+        <v>3.1</v>
+      </c>
+      <c r="N89">
+        <f t="shared" si="3"/>
+        <v>0.31</v>
+      </c>
+      <c r="O89" s="58">
+        <f t="shared" si="4"/>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="P89" s="58">
+        <f t="shared" si="5"/>
+        <v>0.87308644400785873</v>
+      </c>
+    </row>
+    <row r="90" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M90" s="66">
+        <v>3.1</v>
+      </c>
+      <c r="N90">
+        <f t="shared" si="3"/>
+        <v>0.31</v>
+      </c>
+      <c r="O90" s="58">
+        <f t="shared" si="4"/>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="P90" s="58">
+        <f t="shared" si="5"/>
+        <v>0.87308644400785873</v>
+      </c>
+    </row>
+    <row r="91" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M91" s="66">
+        <v>3.1</v>
+      </c>
+      <c r="N91">
+        <f t="shared" si="3"/>
+        <v>0.31</v>
+      </c>
+      <c r="O91" s="58">
+        <f t="shared" si="4"/>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="P91" s="58">
+        <f t="shared" si="5"/>
+        <v>0.87308644400785873</v>
+      </c>
+    </row>
+    <row r="92" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M92" s="66">
+        <v>3.1</v>
+      </c>
+      <c r="N92">
+        <f t="shared" si="3"/>
+        <v>0.31</v>
+      </c>
+      <c r="O92" s="58">
+        <f t="shared" si="4"/>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="P92" s="58">
+        <f t="shared" si="5"/>
+        <v>0.87308644400785873</v>
+      </c>
+    </row>
+    <row r="93" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M93" s="66">
+        <v>3.1</v>
+      </c>
+      <c r="N93">
+        <f t="shared" si="3"/>
+        <v>0.31</v>
+      </c>
+      <c r="O93" s="58">
+        <f t="shared" si="4"/>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="P93" s="58">
+        <f t="shared" si="5"/>
+        <v>0.87308644400785873</v>
+      </c>
+    </row>
+    <row r="94" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M94" s="66">
+        <v>3.1</v>
+      </c>
+      <c r="N94">
+        <f t="shared" si="3"/>
+        <v>0.31</v>
+      </c>
+      <c r="O94" s="58">
+        <f t="shared" si="4"/>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="P94" s="58">
+        <f t="shared" si="5"/>
+        <v>0.87308644400785873</v>
+      </c>
+    </row>
+    <row r="95" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M95" s="66">
+        <v>3.1</v>
+      </c>
+      <c r="N95">
+        <f t="shared" si="3"/>
+        <v>0.31</v>
+      </c>
+      <c r="O95" s="58">
+        <f t="shared" si="4"/>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="P95" s="58">
+        <f t="shared" si="5"/>
+        <v>0.87308644400785873</v>
+      </c>
+    </row>
+    <row r="96" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M96" s="66">
+        <v>3.1</v>
+      </c>
+      <c r="N96">
+        <f t="shared" si="3"/>
+        <v>0.31</v>
+      </c>
+      <c r="O96" s="58">
+        <f t="shared" si="4"/>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="P96" s="58">
+        <f t="shared" si="5"/>
+        <v>0.87308644400785873</v>
+      </c>
+    </row>
+    <row r="97" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M97" s="66">
+        <v>3.1</v>
+      </c>
+      <c r="N97">
+        <f t="shared" si="3"/>
+        <v>0.31</v>
+      </c>
+      <c r="O97" s="58">
+        <f t="shared" si="4"/>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="P97" s="58">
+        <f t="shared" si="5"/>
+        <v>0.87308644400785873</v>
+      </c>
+    </row>
+    <row r="98" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M98" s="66">
+        <v>3.2</v>
+      </c>
+      <c r="N98">
+        <f t="shared" si="3"/>
+        <v>0.32</v>
+      </c>
+      <c r="O98" s="58">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="P98" s="58">
+        <f t="shared" si="5"/>
+        <v>0.90583038637852009</v>
+      </c>
+    </row>
+    <row r="99" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M99" s="66">
+        <v>3.2</v>
+      </c>
+      <c r="N99">
+        <f t="shared" si="3"/>
+        <v>0.32</v>
+      </c>
+      <c r="O99" s="58">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="P99" s="58">
+        <f t="shared" si="5"/>
+        <v>0.90583038637852009</v>
+      </c>
+    </row>
+    <row r="100" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M100" s="66">
+        <v>3.2</v>
+      </c>
+      <c r="N100">
+        <f t="shared" si="3"/>
+        <v>0.32</v>
+      </c>
+      <c r="O100" s="58">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="P100" s="58">
+        <f t="shared" si="5"/>
+        <v>0.90583038637852009</v>
+      </c>
+    </row>
+    <row r="101" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M101" s="66">
+        <v>3.2</v>
+      </c>
+      <c r="N101">
+        <f t="shared" si="3"/>
+        <v>0.32</v>
+      </c>
+      <c r="O101" s="58">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="P101" s="58">
+        <f t="shared" si="5"/>
+        <v>0.90583038637852009</v>
+      </c>
+    </row>
+    <row r="102" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M102" s="66">
+        <v>3.2</v>
+      </c>
+      <c r="N102">
+        <f t="shared" si="3"/>
+        <v>0.32</v>
+      </c>
+      <c r="O102" s="58">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="P102" s="58">
+        <f t="shared" si="5"/>
+        <v>0.90583038637852009</v>
+      </c>
+    </row>
+    <row r="103" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M103" s="66">
+        <v>3.2</v>
+      </c>
+      <c r="N103">
+        <f t="shared" si="3"/>
+        <v>0.32</v>
+      </c>
+      <c r="O103" s="58">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="P103" s="58">
+        <f t="shared" si="5"/>
+        <v>0.90583038637852009</v>
+      </c>
+    </row>
+    <row r="104" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M104" s="66">
+        <v>3.2</v>
+      </c>
+      <c r="N104">
+        <f t="shared" si="3"/>
+        <v>0.32</v>
+      </c>
+      <c r="O104" s="58">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="P104" s="58">
+        <f t="shared" si="5"/>
+        <v>0.90583038637852009</v>
+      </c>
+    </row>
+    <row r="105" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M105" s="66">
+        <v>3.2</v>
+      </c>
+      <c r="N105">
+        <f t="shared" si="3"/>
+        <v>0.32</v>
+      </c>
+      <c r="O105" s="58">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="P105" s="58">
+        <f t="shared" si="5"/>
+        <v>0.90583038637852009</v>
+      </c>
+    </row>
+    <row r="106" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M106" s="66">
+        <v>3.2</v>
+      </c>
+      <c r="N106">
+        <f t="shared" si="3"/>
+        <v>0.32</v>
+      </c>
+      <c r="O106" s="58">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="P106" s="58">
+        <f t="shared" si="5"/>
+        <v>0.90583038637852009</v>
+      </c>
+    </row>
+    <row r="107" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M107" s="66">
+        <v>3.2</v>
+      </c>
+      <c r="N107">
+        <f t="shared" si="3"/>
+        <v>0.32</v>
+      </c>
+      <c r="O107" s="58">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="P107" s="58">
+        <f t="shared" si="5"/>
+        <v>0.90583038637852009</v>
+      </c>
+    </row>
+    <row r="108" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M108" s="66">
+        <v>3.2</v>
+      </c>
+      <c r="N108">
+        <f t="shared" si="3"/>
+        <v>0.32</v>
+      </c>
+      <c r="O108" s="58">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="P108" s="58">
+        <f t="shared" si="5"/>
+        <v>0.90583038637852009</v>
+      </c>
+    </row>
+    <row r="109" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M109" s="66">
+        <v>3.2</v>
+      </c>
+      <c r="N109">
+        <f t="shared" si="3"/>
+        <v>0.32</v>
+      </c>
+      <c r="O109" s="58">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="P109" s="58">
+        <f t="shared" si="5"/>
+        <v>0.90583038637852009</v>
+      </c>
+    </row>
+    <row r="110" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M110" s="66">
+        <v>3.2</v>
+      </c>
+      <c r="N110">
+        <f t="shared" si="3"/>
+        <v>0.32</v>
+      </c>
+      <c r="O110" s="58">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="P110" s="58">
+        <f t="shared" si="5"/>
+        <v>0.90583038637852009</v>
+      </c>
+    </row>
+    <row r="111" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M111" s="66">
+        <v>3.3</v>
+      </c>
+      <c r="N111">
+        <f t="shared" si="3"/>
+        <v>0.32999999999999996</v>
+      </c>
+      <c r="O111" s="58">
+        <f t="shared" si="4"/>
+        <v>0.54166666666666652</v>
+      </c>
+      <c r="P111" s="58">
+        <f t="shared" si="5"/>
+        <v>0.93857432874918145</v>
+      </c>
+    </row>
+    <row r="112" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M112" s="66">
+        <v>3.3</v>
+      </c>
+      <c r="N112">
+        <f t="shared" si="3"/>
+        <v>0.32999999999999996</v>
+      </c>
+      <c r="O112" s="58">
+        <f t="shared" si="4"/>
+        <v>0.54166666666666652</v>
+      </c>
+      <c r="P112" s="58">
+        <f t="shared" si="5"/>
+        <v>0.93857432874918145</v>
+      </c>
+    </row>
+    <row r="113" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M113" s="66">
+        <v>3.3</v>
+      </c>
+      <c r="N113">
+        <f t="shared" si="3"/>
+        <v>0.32999999999999996</v>
+      </c>
+      <c r="O113" s="58">
+        <f t="shared" si="4"/>
+        <v>0.54166666666666652</v>
+      </c>
+      <c r="P113" s="58">
+        <f t="shared" si="5"/>
+        <v>0.93857432874918145</v>
+      </c>
+    </row>
+    <row r="114" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M114" s="66">
+        <v>3.3</v>
+      </c>
+      <c r="N114">
+        <f t="shared" si="3"/>
+        <v>0.32999999999999996</v>
+      </c>
+      <c r="O114" s="58">
+        <f t="shared" si="4"/>
+        <v>0.54166666666666652</v>
+      </c>
+      <c r="P114" s="58">
+        <f t="shared" si="5"/>
+        <v>0.93857432874918145</v>
+      </c>
+    </row>
+    <row r="115" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M115" s="66">
+        <v>3.3</v>
+      </c>
+      <c r="N115">
+        <f t="shared" si="3"/>
+        <v>0.32999999999999996</v>
+      </c>
+      <c r="O115" s="58">
+        <f t="shared" si="4"/>
+        <v>0.54166666666666652</v>
+      </c>
+      <c r="P115" s="58">
+        <f t="shared" si="5"/>
+        <v>0.93857432874918145</v>
+      </c>
+    </row>
+    <row r="116" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M116" s="66">
+        <v>3.3</v>
+      </c>
+      <c r="N116">
+        <f t="shared" si="3"/>
+        <v>0.32999999999999996</v>
+      </c>
+      <c r="O116" s="58">
+        <f t="shared" si="4"/>
+        <v>0.54166666666666652</v>
+      </c>
+      <c r="P116" s="58">
+        <f t="shared" si="5"/>
+        <v>0.93857432874918145</v>
+      </c>
+    </row>
+    <row r="117" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M117" s="66">
+        <v>3.4</v>
+      </c>
+      <c r="N117">
+        <f t="shared" si="3"/>
+        <v>0.33999999999999997</v>
+      </c>
+      <c r="O117" s="58">
+        <f t="shared" si="4"/>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="P117" s="58">
+        <f t="shared" si="5"/>
+        <v>0.97131827111984292</v>
+      </c>
+    </row>
+    <row r="118" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M118" s="66">
+        <v>3.4</v>
+      </c>
+      <c r="N118">
+        <f t="shared" si="3"/>
+        <v>0.33999999999999997</v>
+      </c>
+      <c r="O118" s="58">
+        <f t="shared" si="4"/>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="P118" s="58">
+        <f t="shared" si="5"/>
+        <v>0.97131827111984292</v>
+      </c>
+    </row>
+    <row r="119" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M119" s="66">
+        <v>3.4</v>
+      </c>
+      <c r="N119">
+        <f t="shared" si="3"/>
+        <v>0.33999999999999997</v>
+      </c>
+      <c r="O119" s="58">
+        <f t="shared" si="4"/>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="P119" s="58">
+        <f t="shared" si="5"/>
+        <v>0.97131827111984292</v>
+      </c>
+    </row>
+    <row r="120" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M120" s="66">
+        <v>3.4</v>
+      </c>
+      <c r="N120">
+        <f t="shared" si="3"/>
+        <v>0.33999999999999997</v>
+      </c>
+      <c r="O120" s="58">
+        <f t="shared" si="4"/>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="P120" s="58">
+        <f t="shared" si="5"/>
+        <v>0.97131827111984292</v>
+      </c>
+    </row>
+    <row r="121" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M121" s="66">
+        <v>3.4</v>
+      </c>
+      <c r="N121">
+        <f t="shared" si="3"/>
+        <v>0.33999999999999997</v>
+      </c>
+      <c r="O121" s="58">
+        <f t="shared" si="4"/>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="P121" s="58">
+        <f t="shared" si="5"/>
+        <v>0.97131827111984292</v>
+      </c>
+    </row>
+    <row r="122" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M122" s="66">
+        <v>3.4</v>
+      </c>
+      <c r="N122">
+        <f t="shared" si="3"/>
+        <v>0.33999999999999997</v>
+      </c>
+      <c r="O122" s="58">
+        <f t="shared" si="4"/>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="P122" s="58">
+        <f t="shared" si="5"/>
+        <v>0.97131827111984292</v>
+      </c>
+    </row>
+    <row r="123" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M123" s="66">
+        <v>3.4</v>
+      </c>
+      <c r="N123">
+        <f t="shared" si="3"/>
+        <v>0.33999999999999997</v>
+      </c>
+      <c r="O123" s="58">
+        <f t="shared" si="4"/>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="P123" s="58">
+        <f t="shared" si="5"/>
+        <v>0.97131827111984292</v>
+      </c>
+    </row>
+    <row r="124" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M124" s="66">
+        <v>3.4</v>
+      </c>
+      <c r="N124">
+        <f t="shared" si="3"/>
+        <v>0.33999999999999997</v>
+      </c>
+      <c r="O124" s="58">
+        <f t="shared" si="4"/>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="P124" s="58">
+        <f t="shared" si="5"/>
+        <v>0.97131827111984292</v>
+      </c>
+    </row>
+    <row r="125" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M125" s="66">
+        <v>3.4</v>
+      </c>
+      <c r="N125">
+        <f t="shared" si="3"/>
+        <v>0.33999999999999997</v>
+      </c>
+      <c r="O125" s="58">
+        <f t="shared" si="4"/>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="P125" s="58">
+        <f t="shared" si="5"/>
+        <v>0.97131827111984292</v>
+      </c>
+    </row>
+    <row r="126" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M126" s="66">
+        <v>3.4</v>
+      </c>
+      <c r="N126">
+        <f t="shared" si="3"/>
+        <v>0.33999999999999997</v>
+      </c>
+      <c r="O126" s="58">
+        <f t="shared" si="4"/>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="P126" s="58">
+        <f t="shared" si="5"/>
+        <v>0.97131827111984292</v>
+      </c>
+    </row>
+    <row r="127" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M127" s="66">
+        <v>3.4</v>
+      </c>
+      <c r="N127">
+        <f t="shared" si="3"/>
+        <v>0.33999999999999997</v>
+      </c>
+      <c r="O127" s="58">
+        <f t="shared" si="4"/>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="P127" s="58">
+        <f t="shared" si="5"/>
+        <v>0.97131827111984292</v>
+      </c>
+    </row>
+    <row r="128" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M128" s="66">
+        <v>3.4</v>
+      </c>
+      <c r="N128">
+        <f t="shared" si="3"/>
+        <v>0.33999999999999997</v>
+      </c>
+      <c r="O128" s="58">
+        <f t="shared" si="4"/>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="P128" s="58">
+        <f t="shared" si="5"/>
+        <v>0.97131827111984292</v>
+      </c>
+    </row>
+    <row r="129" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M129" s="66">
+        <v>3.5</v>
+      </c>
+      <c r="N129">
+        <f t="shared" si="3"/>
+        <v>0.35</v>
+      </c>
+      <c r="O129" s="58">
+        <f t="shared" si="4"/>
+        <v>0.62499999999999989</v>
+      </c>
+      <c r="P129" s="58">
+        <f t="shared" si="5"/>
+        <v>1.0040622134905044</v>
+      </c>
+    </row>
+    <row r="130" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M130" s="66">
+        <v>3.5</v>
+      </c>
+      <c r="N130">
+        <f t="shared" si="3"/>
+        <v>0.35</v>
+      </c>
+      <c r="O130" s="58">
+        <f t="shared" si="4"/>
+        <v>0.62499999999999989</v>
+      </c>
+      <c r="P130" s="58">
+        <f t="shared" si="5"/>
+        <v>1.0040622134905044</v>
+      </c>
+    </row>
+    <row r="131" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M131" s="66">
+        <v>3.5</v>
+      </c>
+      <c r="N131">
+        <f t="shared" si="3"/>
+        <v>0.35</v>
+      </c>
+      <c r="O131" s="58">
+        <f t="shared" si="4"/>
+        <v>0.62499999999999989</v>
+      </c>
+      <c r="P131" s="58">
+        <f t="shared" si="5"/>
+        <v>1.0040622134905044</v>
+      </c>
+    </row>
+    <row r="132" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M132" s="66">
+        <v>3.5</v>
+      </c>
+      <c r="N132">
+        <f t="shared" ref="N132:N152" si="6">M132/10</f>
+        <v>0.35</v>
+      </c>
+      <c r="O132" s="58">
+        <f t="shared" ref="O132:O152" si="7">((M132-2)/(4.4-2))*(1-0)+0</f>
+        <v>0.62499999999999989</v>
+      </c>
+      <c r="P132" s="58">
+        <f t="shared" ref="P132:P152" si="8">(M132-0.433594)/3.054</f>
+        <v>1.0040622134905044</v>
+      </c>
+    </row>
+    <row r="133" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M133" s="66">
+        <v>3.5</v>
+      </c>
+      <c r="N133">
+        <f t="shared" si="6"/>
+        <v>0.35</v>
+      </c>
+      <c r="O133" s="58">
+        <f t="shared" si="7"/>
+        <v>0.62499999999999989</v>
+      </c>
+      <c r="P133" s="58">
+        <f t="shared" si="8"/>
+        <v>1.0040622134905044</v>
+      </c>
+    </row>
+    <row r="134" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M134" s="66">
+        <v>3.5</v>
+      </c>
+      <c r="N134">
+        <f t="shared" si="6"/>
+        <v>0.35</v>
+      </c>
+      <c r="O134" s="58">
+        <f t="shared" si="7"/>
+        <v>0.62499999999999989</v>
+      </c>
+      <c r="P134" s="58">
+        <f t="shared" si="8"/>
+        <v>1.0040622134905044</v>
+      </c>
+    </row>
+    <row r="135" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M135" s="66">
+        <v>3.6</v>
+      </c>
+      <c r="N135">
+        <f t="shared" si="6"/>
+        <v>0.36</v>
+      </c>
+      <c r="O135" s="58">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="P135" s="58">
+        <f t="shared" si="8"/>
+        <v>1.0368061558611659</v>
+      </c>
+    </row>
+    <row r="136" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M136" s="66">
+        <v>3.6</v>
+      </c>
+      <c r="N136">
+        <f t="shared" si="6"/>
+        <v>0.36</v>
+      </c>
+      <c r="O136" s="58">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="P136" s="58">
+        <f t="shared" si="8"/>
+        <v>1.0368061558611659</v>
+      </c>
+    </row>
+    <row r="137" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M137" s="66">
+        <v>3.6</v>
+      </c>
+      <c r="N137">
+        <f t="shared" si="6"/>
+        <v>0.36</v>
+      </c>
+      <c r="O137" s="58">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="P137" s="58">
+        <f t="shared" si="8"/>
+        <v>1.0368061558611659</v>
+      </c>
+    </row>
+    <row r="138" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M138" s="66">
+        <v>3.7</v>
+      </c>
+      <c r="N138">
+        <f t="shared" si="6"/>
+        <v>0.37</v>
+      </c>
+      <c r="O138" s="58">
+        <f t="shared" si="7"/>
+        <v>0.70833333333333326</v>
+      </c>
+      <c r="P138" s="58">
+        <f t="shared" si="8"/>
+        <v>1.0695500982318273</v>
+      </c>
+    </row>
+    <row r="139" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M139" s="66">
+        <v>3.7</v>
+      </c>
+      <c r="N139">
+        <f t="shared" si="6"/>
+        <v>0.37</v>
+      </c>
+      <c r="O139" s="58">
+        <f t="shared" si="7"/>
+        <v>0.70833333333333326</v>
+      </c>
+      <c r="P139" s="58">
+        <f t="shared" si="8"/>
+        <v>1.0695500982318273</v>
+      </c>
+    </row>
+    <row r="140" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M140" s="66">
+        <v>3.7</v>
+      </c>
+      <c r="N140">
+        <f t="shared" si="6"/>
+        <v>0.37</v>
+      </c>
+      <c r="O140" s="58">
+        <f t="shared" si="7"/>
+        <v>0.70833333333333326</v>
+      </c>
+      <c r="P140" s="58">
+        <f t="shared" si="8"/>
+        <v>1.0695500982318273</v>
+      </c>
+    </row>
+    <row r="141" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M141" s="66">
+        <v>3.8</v>
+      </c>
+      <c r="N141">
+        <f t="shared" si="6"/>
+        <v>0.38</v>
+      </c>
+      <c r="O141" s="58">
+        <f t="shared" si="7"/>
+        <v>0.74999999999999978</v>
+      </c>
+      <c r="P141" s="58">
+        <f t="shared" si="8"/>
+        <v>1.1022940406024886</v>
+      </c>
+    </row>
+    <row r="142" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M142" s="66">
+        <v>3.8</v>
+      </c>
+      <c r="N142">
+        <f t="shared" si="6"/>
+        <v>0.38</v>
+      </c>
+      <c r="O142" s="58">
+        <f t="shared" si="7"/>
+        <v>0.74999999999999978</v>
+      </c>
+      <c r="P142" s="58">
+        <f t="shared" si="8"/>
+        <v>1.1022940406024886</v>
+      </c>
+    </row>
+    <row r="143" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M143" s="66">
+        <v>3.8</v>
+      </c>
+      <c r="N143">
+        <f t="shared" si="6"/>
+        <v>0.38</v>
+      </c>
+      <c r="O143" s="58">
+        <f t="shared" si="7"/>
+        <v>0.74999999999999978</v>
+      </c>
+      <c r="P143" s="58">
+        <f t="shared" si="8"/>
+        <v>1.1022940406024886</v>
+      </c>
+    </row>
+    <row r="144" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M144" s="66">
+        <v>3.8</v>
+      </c>
+      <c r="N144">
+        <f t="shared" si="6"/>
+        <v>0.38</v>
+      </c>
+      <c r="O144" s="58">
+        <f t="shared" si="7"/>
+        <v>0.74999999999999978</v>
+      </c>
+      <c r="P144" s="58">
+        <f t="shared" si="8"/>
+        <v>1.1022940406024886</v>
+      </c>
+    </row>
+    <row r="145" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M145" s="66">
+        <v>3.8</v>
+      </c>
+      <c r="N145">
+        <f t="shared" si="6"/>
+        <v>0.38</v>
+      </c>
+      <c r="O145" s="58">
+        <f t="shared" si="7"/>
+        <v>0.74999999999999978</v>
+      </c>
+      <c r="P145" s="58">
+        <f t="shared" si="8"/>
+        <v>1.1022940406024886</v>
+      </c>
+    </row>
+    <row r="146" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M146" s="66">
+        <v>3.8</v>
+      </c>
+      <c r="N146">
+        <f t="shared" si="6"/>
+        <v>0.38</v>
+      </c>
+      <c r="O146" s="58">
+        <f t="shared" si="7"/>
+        <v>0.74999999999999978</v>
+      </c>
+      <c r="P146" s="58">
+        <f t="shared" si="8"/>
+        <v>1.1022940406024886</v>
+      </c>
+    </row>
+    <row r="147" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M147" s="66">
+        <v>3.9</v>
+      </c>
+      <c r="N147">
+        <f t="shared" si="6"/>
+        <v>0.39</v>
+      </c>
+      <c r="O147" s="58">
+        <f t="shared" si="7"/>
+        <v>0.79166666666666652</v>
+      </c>
+      <c r="P147" s="58">
+        <f t="shared" si="8"/>
+        <v>1.1350379829731501</v>
+      </c>
+    </row>
+    <row r="148" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M148" s="66">
+        <v>3.9</v>
+      </c>
+      <c r="N148">
+        <f t="shared" si="6"/>
+        <v>0.39</v>
+      </c>
+      <c r="O148" s="58">
+        <f t="shared" si="7"/>
+        <v>0.79166666666666652</v>
+      </c>
+      <c r="P148" s="58">
+        <f t="shared" si="8"/>
+        <v>1.1350379829731501</v>
+      </c>
+    </row>
+    <row r="149" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M149" s="66">
+        <v>4</v>
+      </c>
+      <c r="N149">
+        <f t="shared" si="6"/>
+        <v>0.4</v>
+      </c>
+      <c r="O149" s="58">
+        <f t="shared" si="7"/>
+        <v>0.83333333333333326</v>
+      </c>
+      <c r="P149" s="58">
+        <f t="shared" si="8"/>
+        <v>1.1677819253438115</v>
+      </c>
+    </row>
+    <row r="150" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M150" s="66">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N150">
+        <f t="shared" si="6"/>
+        <v>0.41</v>
+      </c>
+      <c r="O150" s="58">
+        <f t="shared" si="7"/>
+        <v>0.87499999999999978</v>
+      </c>
+      <c r="P150" s="58">
+        <f t="shared" si="8"/>
+        <v>1.2005258677144728</v>
+      </c>
+    </row>
+    <row r="151" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M151" s="66">
+        <v>4.2</v>
+      </c>
+      <c r="N151">
+        <f t="shared" si="6"/>
+        <v>0.42000000000000004</v>
+      </c>
+      <c r="O151" s="58">
+        <f t="shared" si="7"/>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="P151" s="58">
+        <f t="shared" si="8"/>
+        <v>1.2332698100851345</v>
+      </c>
+    </row>
+    <row r="152" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M152" s="66">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="N152">
+        <f t="shared" si="6"/>
+        <v>0.44000000000000006</v>
+      </c>
+      <c r="O152" s="58">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="P152" s="58">
+        <f t="shared" si="8"/>
+        <v>1.2987576948264574</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M3:M152">
+    <sortCondition ref="M3:M152"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -9692,15 +12467,15 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="70" t="s">
         <v>228</v>
       </c>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">

</xml_diff>

<commit_message>
lab 4 homework 4
</commit_message>
<xml_diff>
--- a/COMP300-HomeworkProblems-SP20.xlsx
+++ b/COMP300-HomeworkProblems-SP20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benlo\DataMining2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6B2BF9-D7B8-40D0-ADF7-1FD451562A90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF2537F-30E6-4BC2-A02B-03A11461C343}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3105" yWindow="3105" windowWidth="7500" windowHeight="6000" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HW Index" sheetId="38" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="459">
   <si>
     <t>Mean</t>
   </si>
@@ -771,9 +771,6 @@
     <t>For each Chemist:</t>
   </si>
   <si>
-    <t>A  chemical research company runs multiple projects.  Each project is headquartered in specific region.  Projects require chemists to work on them, and equipment must be assigned to those chemists for specific projects.  The company maintains many categories of equipment, much of it quite expensive.  Therefore, the company maintains records of the number of hours that a specific piece of equipment is checked out to a specific chemist for a specific project.  In addition, the charge to the project varies, depending upon the project, the chemist and the equipment.</t>
-  </si>
-  <si>
     <t>The following attributes are  stored in the data warehouse for each instance of equipment assignment:</t>
   </si>
   <si>
@@ -1521,6 +1518,89 @@
   <si>
     <t xml:space="preserve">with the paramters of 0 to 1 for the new values are distributed similarly to the unnormailzed data. one issue that didn’t occur in this dataset, but can with others, is if there is an outlier it will stay an outlyer and skew the data. </t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A  chemical research company runs multiple projects.  Each project is headquartered in specific region.  Projects require chemists to work on them, and equipment must be assigned to those chemists for specific projects.  The company maintains many categories of equipment, much of it quite expensive.  Therefore, the company maintains records of the </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>number of hours that a specific piece of equipment is checked out to a specific chemist for a specific project</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.  In addition, the charge to the project varies, depending upon the project, the chemist and the equipment.</t>
+    </r>
+  </si>
+  <si>
+    <t>num_hours</t>
+  </si>
+  <si>
+    <t>charge_per_hr</t>
+  </si>
+  <si>
+    <t>chemist</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>equipment</t>
+  </si>
+  <si>
+    <t>fact table</t>
+  </si>
+  <si>
+    <t>Chemist_key</t>
+  </si>
+  <si>
+    <t>Project_key</t>
+  </si>
+  <si>
+    <t>Equipment_key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roll up to university and slice on course comp 300 </t>
+  </si>
+  <si>
+    <t>roll up to university and slice on course comp 300 slice on instructor #007</t>
+  </si>
+  <si>
+    <t>roll up to university and roll up to department and slice on CS department</t>
+  </si>
+  <si>
+    <t>roll up to major and roll up to year and dice on math and 2013</t>
+  </si>
+  <si>
+    <t>roll up to year and roll up to university and slice on 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drill down to base cuboid </t>
+  </si>
+  <si>
+    <t xml:space="preserve">roll up to department and drill down to student_id and slice on English </t>
+  </si>
+  <si>
+    <t>roll up to year and slice on 2012</t>
+  </si>
+  <si>
+    <t>roll up to year and roll up to university and slice on 2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T = </t>
+  </si>
 </sst>
 </file>
 
@@ -1530,7 +1610,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1655,6 +1735,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1682,7 +1770,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1837,12 +1925,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1988,15 +2087,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3318,6 +3419,170 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1104900</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C88150C6-1053-4E6C-BA77-945E0DCF33CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1485900" y="7820025"/>
+          <a:ext cx="1028700" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1114425</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AAE28C9-3A19-4664-BA3C-E628D629DB20}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1466850" y="8391525"/>
+          <a:ext cx="1057275" cy="590550"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E06C5582-428C-4F00-BEAF-017BBC9DF9BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3905250" y="7772400"/>
+          <a:ext cx="1066800" cy="847725"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -3374,7 +3639,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -3445,7 +3710,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3564,7 +3829,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3939,7 +4204,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3977,10 +4242,10 @@
         <v>213</v>
       </c>
       <c r="B9" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3988,7 +4253,7 @@
         <v>214</v>
       </c>
       <c r="B10" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3996,10 +4261,10 @@
         <v>215</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -4012,7 +4277,7 @@
     </row>
     <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B13" t="s">
         <v>218</v>
@@ -4023,10 +4288,10 @@
         <v>219</v>
       </c>
       <c r="B14" t="s">
+        <v>385</v>
+      </c>
+      <c r="D14" t="s">
         <v>386</v>
-      </c>
-      <c r="D14" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -4037,17 +4302,17 @@
         <v>221</v>
       </c>
       <c r="D15" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -4089,7 +4354,7 @@
         <v>115</v>
       </c>
       <c r="B6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F6" t="s">
         <v>116</v>
@@ -4100,7 +4365,7 @@
         <v>117</v>
       </c>
       <c r="B7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F7" t="s">
         <v>118</v>
@@ -4111,7 +4376,7 @@
         <v>119</v>
       </c>
       <c r="B8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -4119,7 +4384,7 @@
         <v>120</v>
       </c>
       <c r="B9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -4127,7 +4392,7 @@
         <v>121</v>
       </c>
       <c r="B10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -4135,22 +4400,22 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -4158,7 +4423,7 @@
         <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -4166,7 +4431,7 @@
         <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -4174,19 +4439,19 @@
         <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -4211,23 +4476,23 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D4" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>276</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D5" s="24">
         <v>1500</v>
@@ -4238,7 +4503,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D6" s="24">
         <v>2000</v>
@@ -4257,7 +4522,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -4290,7 +4555,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -4300,108 +4565,108 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D22" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D23" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D24" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D25" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="36" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="37" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C38" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="37" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C39" s="37" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="41" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="37" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="43" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="37" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -4436,22 +4701,22 @@
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -4471,7 +4736,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -4496,7 +4761,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -4506,25 +4771,25 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>333</v>
+      </c>
+      <c r="C21" t="s">
         <v>334</v>
-      </c>
-      <c r="C21" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H25" s="41">
         <f>((-9/14) * LOG((9/14),2)) - ((5/14)*LOG((5/14),2))</f>
@@ -4533,7 +4798,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -4541,43 +4806,43 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="33" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="B35" s="26" t="s">
         <v>342</v>
       </c>
-      <c r="B35" s="26" t="s">
+      <c r="C35" s="40" t="s">
         <v>343</v>
       </c>
-      <c r="C35" s="40" t="s">
+      <c r="D35" s="40" t="s">
         <v>344</v>
       </c>
-      <c r="D35" s="40" t="s">
+      <c r="E35" s="40" t="s">
+        <v>367</v>
+      </c>
+      <c r="F35" s="40" t="s">
         <v>345</v>
       </c>
-      <c r="E35" s="40" t="s">
-        <v>368</v>
-      </c>
-      <c r="F35" s="40" t="s">
+      <c r="G35" s="40" t="s">
         <v>346</v>
       </c>
-      <c r="G35" s="40" t="s">
+      <c r="H35" s="43" t="s">
         <v>347</v>
-      </c>
-      <c r="H35" s="43" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B36" s="24">
         <v>1</v>
@@ -4605,7 +4870,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B37" s="24">
         <v>2</v>
@@ -4633,7 +4898,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="44" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B38" s="24">
         <v>3</v>
@@ -4658,7 +4923,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="45" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B39" s="34"/>
       <c r="C39" s="34"/>
@@ -4692,14 +4957,14 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C43" s="34"/>
       <c r="D43" s="34"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="41" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B44" s="41"/>
       <c r="C44" s="41"/>
@@ -4716,7 +4981,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="25" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B46" s="25"/>
       <c r="C46" s="25"/>
@@ -4724,7 +4989,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B47" s="25"/>
       <c r="C47" s="25"/>
@@ -4732,38 +4997,38 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="33" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="26" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B49" s="26" t="s">
+        <v>342</v>
+      </c>
+      <c r="C49" s="40" t="s">
         <v>343</v>
       </c>
-      <c r="C49" s="40" t="s">
+      <c r="D49" s="40" t="s">
         <v>344</v>
       </c>
-      <c r="D49" s="40" t="s">
+      <c r="E49" s="40" t="s">
+        <v>367</v>
+      </c>
+      <c r="F49" s="40" t="s">
         <v>345</v>
       </c>
-      <c r="E49" s="40" t="s">
-        <v>368</v>
-      </c>
-      <c r="F49" s="40" t="s">
+      <c r="G49" s="40" t="s">
         <v>346</v>
       </c>
-      <c r="G49" s="40" t="s">
+      <c r="H49" s="43" t="s">
         <v>347</v>
-      </c>
-      <c r="H49" s="43" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="24" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B50" s="24">
         <v>1</v>
@@ -4791,7 +5056,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="24" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B51" s="24">
         <v>2</v>
@@ -4819,7 +5084,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="44" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B52" s="24">
         <v>3</v>
@@ -4879,14 +5144,14 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C57" s="34"/>
       <c r="D57" s="34"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="46" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B58" s="46"/>
       <c r="C58" s="46"/>
@@ -4913,7 +5178,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="27" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B61" s="25"/>
       <c r="C61" s="25"/>
@@ -4927,30 +5192,30 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="26" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B63" s="26" t="s">
+        <v>342</v>
+      </c>
+      <c r="C63" s="40" t="s">
         <v>343</v>
       </c>
-      <c r="C63" s="40" t="s">
+      <c r="D63" s="40" t="s">
         <v>344</v>
       </c>
-      <c r="D63" s="40" t="s">
-        <v>345</v>
-      </c>
       <c r="E63" s="40" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F63" s="47" t="s">
+        <v>363</v>
+      </c>
+      <c r="G63" s="40" t="s">
         <v>364</v>
-      </c>
-      <c r="G63" s="40" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="24" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B64" s="24">
         <v>1</v>
@@ -4976,7 +5241,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="24" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B65" s="24">
         <v>2</v>
@@ -5002,7 +5267,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="44" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B66" s="24">
         <v>3</v>
@@ -5042,7 +5307,7 @@
       <c r="C68" s="25"/>
       <c r="D68" s="25"/>
       <c r="E68" s="71" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F68" s="71"/>
       <c r="G68" s="48">
@@ -5072,7 +5337,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="72" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B72" s="71"/>
       <c r="C72" s="71"/>
@@ -5145,7 +5410,7 @@
     </row>
     <row r="2" spans="1:4" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B2" s="38"/>
       <c r="C2" s="38"/>
@@ -5153,7 +5418,7 @@
     </row>
     <row r="3" spans="1:4" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="39" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -5161,12 +5426,12 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5186,52 +5451,52 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -5284,7 +5549,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B42" s="25"/>
       <c r="C42" s="25"/>
@@ -5292,12 +5557,12 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -5338,7 +5603,7 @@
         <v>133</v>
       </c>
       <c r="K2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -5348,24 +5613,24 @@
     </row>
     <row r="4" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B4" s="56">
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B5" s="56">
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6028,7 +6293,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6190,7 +6455,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6394,13 +6659,13 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="55" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B49" s="11">
         <v>5</v>
       </c>
       <c r="D49" s="55" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E49" s="11">
         <v>5</v>
@@ -6408,7 +6673,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6872,12 +7137,12 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7118,7 +7383,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -7304,31 +7569,31 @@
       <c r="B50" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="C50" s="74" t="s">
+      <c r="C50" s="73" t="s">
         <v>174</v>
       </c>
-      <c r="D50" s="74"/>
-      <c r="E50" s="74"/>
-      <c r="F50" s="74"/>
-      <c r="G50" s="74"/>
+      <c r="D50" s="73"/>
+      <c r="E50" s="73"/>
+      <c r="F50" s="73"/>
+      <c r="G50" s="73"/>
       <c r="H50" s="26" t="s">
         <v>175</v>
       </c>
       <c r="I50" s="26"/>
-      <c r="J50" s="74" t="s">
+      <c r="J50" s="73" t="s">
         <v>176</v>
       </c>
-      <c r="K50" s="74"/>
+      <c r="K50" s="73"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B51" s="24">
         <v>4</v>
       </c>
-      <c r="C51" s="73"/>
-      <c r="D51" s="73"/>
-      <c r="E51" s="73"/>
-      <c r="F51" s="73"/>
-      <c r="G51" s="73"/>
+      <c r="C51" s="74"/>
+      <c r="D51" s="74"/>
+      <c r="E51" s="74"/>
+      <c r="F51" s="74"/>
+      <c r="G51" s="74"/>
       <c r="H51" s="75"/>
       <c r="I51" s="75"/>
       <c r="J51" s="75"/>
@@ -7338,11 +7603,11 @@
       <c r="B52" s="24">
         <v>5</v>
       </c>
-      <c r="C52" s="73"/>
-      <c r="D52" s="73"/>
-      <c r="E52" s="73"/>
-      <c r="F52" s="73"/>
-      <c r="G52" s="73"/>
+      <c r="C52" s="74"/>
+      <c r="D52" s="74"/>
+      <c r="E52" s="74"/>
+      <c r="F52" s="74"/>
+      <c r="G52" s="74"/>
       <c r="H52" s="75"/>
       <c r="I52" s="75"/>
       <c r="J52" s="75"/>
@@ -7352,11 +7617,11 @@
       <c r="B53" s="24">
         <v>6</v>
       </c>
-      <c r="C53" s="73"/>
-      <c r="D53" s="73"/>
-      <c r="E53" s="73"/>
-      <c r="F53" s="73"/>
-      <c r="G53" s="73"/>
+      <c r="C53" s="74"/>
+      <c r="D53" s="74"/>
+      <c r="E53" s="74"/>
+      <c r="F53" s="74"/>
+      <c r="G53" s="74"/>
       <c r="H53" s="75"/>
       <c r="I53" s="75"/>
       <c r="J53" s="75"/>
@@ -7389,61 +7654,61 @@
       <c r="B61" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="C61" s="74" t="s">
+      <c r="C61" s="73" t="s">
         <v>182</v>
       </c>
-      <c r="D61" s="74"/>
-      <c r="E61" s="74"/>
-      <c r="F61" s="74"/>
-      <c r="G61" s="74"/>
-      <c r="H61" s="74"/>
-      <c r="I61" s="74"/>
-      <c r="J61" s="74" t="s">
+      <c r="D61" s="73"/>
+      <c r="E61" s="73"/>
+      <c r="F61" s="73"/>
+      <c r="G61" s="73"/>
+      <c r="H61" s="73"/>
+      <c r="I61" s="73"/>
+      <c r="J61" s="73" t="s">
         <v>183</v>
       </c>
-      <c r="K61" s="74"/>
+      <c r="K61" s="73"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B62" s="24">
         <v>6</v>
       </c>
-      <c r="C62" s="73"/>
-      <c r="D62" s="73"/>
-      <c r="E62" s="73"/>
-      <c r="F62" s="73"/>
-      <c r="G62" s="73"/>
-      <c r="H62" s="73"/>
-      <c r="I62" s="73"/>
-      <c r="J62" s="73"/>
-      <c r="K62" s="73"/>
+      <c r="C62" s="74"/>
+      <c r="D62" s="74"/>
+      <c r="E62" s="74"/>
+      <c r="F62" s="74"/>
+      <c r="G62" s="74"/>
+      <c r="H62" s="74"/>
+      <c r="I62" s="74"/>
+      <c r="J62" s="74"/>
+      <c r="K62" s="74"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B63" s="24">
         <v>5</v>
       </c>
-      <c r="C63" s="73"/>
-      <c r="D63" s="73"/>
-      <c r="E63" s="73"/>
-      <c r="F63" s="73"/>
-      <c r="G63" s="73"/>
-      <c r="H63" s="73"/>
-      <c r="I63" s="73"/>
-      <c r="J63" s="73"/>
-      <c r="K63" s="73"/>
+      <c r="C63" s="74"/>
+      <c r="D63" s="74"/>
+      <c r="E63" s="74"/>
+      <c r="F63" s="74"/>
+      <c r="G63" s="74"/>
+      <c r="H63" s="74"/>
+      <c r="I63" s="74"/>
+      <c r="J63" s="74"/>
+      <c r="K63" s="74"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B64" s="24">
         <v>4</v>
       </c>
-      <c r="C64" s="73"/>
-      <c r="D64" s="73"/>
-      <c r="E64" s="73"/>
-      <c r="F64" s="73"/>
-      <c r="G64" s="73"/>
-      <c r="H64" s="73"/>
-      <c r="I64" s="73"/>
-      <c r="J64" s="73"/>
-      <c r="K64" s="73"/>
+      <c r="C64" s="74"/>
+      <c r="D64" s="74"/>
+      <c r="E64" s="74"/>
+      <c r="F64" s="74"/>
+      <c r="G64" s="74"/>
+      <c r="H64" s="74"/>
+      <c r="I64" s="74"/>
+      <c r="J64" s="74"/>
+      <c r="K64" s="74"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
@@ -7481,19 +7746,19 @@
       <c r="C74" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="D74" s="74" t="s">
+      <c r="D74" s="73" t="s">
         <v>191</v>
       </c>
-      <c r="E74" s="74"/>
-      <c r="F74" s="74"/>
-      <c r="G74" s="74"/>
-      <c r="H74" s="74"/>
-      <c r="I74" s="74"/>
-      <c r="J74" s="74" t="s">
+      <c r="E74" s="73"/>
+      <c r="F74" s="73"/>
+      <c r="G74" s="73"/>
+      <c r="H74" s="73"/>
+      <c r="I74" s="73"/>
+      <c r="J74" s="73" t="s">
         <v>192</v>
       </c>
-      <c r="K74" s="74"/>
-      <c r="L74" s="74"/>
+      <c r="K74" s="73"/>
+      <c r="L74" s="73"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B75" s="29" t="s">
@@ -7502,15 +7767,15 @@
       <c r="C75" s="24">
         <v>1</v>
       </c>
-      <c r="D75" s="73"/>
-      <c r="E75" s="73"/>
-      <c r="F75" s="73"/>
-      <c r="G75" s="73"/>
-      <c r="H75" s="73"/>
-      <c r="I75" s="73"/>
-      <c r="J75" s="73"/>
-      <c r="K75" s="73"/>
-      <c r="L75" s="73"/>
+      <c r="D75" s="74"/>
+      <c r="E75" s="74"/>
+      <c r="F75" s="74"/>
+      <c r="G75" s="74"/>
+      <c r="H75" s="74"/>
+      <c r="I75" s="74"/>
+      <c r="J75" s="74"/>
+      <c r="K75" s="74"/>
+      <c r="L75" s="74"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B76" s="29" t="s">
@@ -7519,15 +7784,15 @@
       <c r="C76" s="24">
         <v>1</v>
       </c>
-      <c r="D76" s="73"/>
-      <c r="E76" s="73"/>
-      <c r="F76" s="73"/>
-      <c r="G76" s="73"/>
-      <c r="H76" s="73"/>
-      <c r="I76" s="73"/>
-      <c r="J76" s="73"/>
-      <c r="K76" s="73"/>
-      <c r="L76" s="73"/>
+      <c r="D76" s="74"/>
+      <c r="E76" s="74"/>
+      <c r="F76" s="74"/>
+      <c r="G76" s="74"/>
+      <c r="H76" s="74"/>
+      <c r="I76" s="74"/>
+      <c r="J76" s="74"/>
+      <c r="K76" s="74"/>
+      <c r="L76" s="74"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B77" s="29" t="s">
@@ -7536,15 +7801,15 @@
       <c r="C77" s="24">
         <v>0</v>
       </c>
-      <c r="D77" s="73"/>
-      <c r="E77" s="73"/>
-      <c r="F77" s="73"/>
-      <c r="G77" s="73"/>
-      <c r="H77" s="73"/>
-      <c r="I77" s="73"/>
-      <c r="J77" s="73"/>
-      <c r="K77" s="73"/>
-      <c r="L77" s="73"/>
+      <c r="D77" s="74"/>
+      <c r="E77" s="74"/>
+      <c r="F77" s="74"/>
+      <c r="G77" s="74"/>
+      <c r="H77" s="74"/>
+      <c r="I77" s="74"/>
+      <c r="J77" s="74"/>
+      <c r="K77" s="74"/>
+      <c r="L77" s="74"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B78" s="29" t="s">
@@ -7553,15 +7818,15 @@
       <c r="C78" s="24">
         <v>0.19214789423111006</v>
       </c>
-      <c r="D78" s="73"/>
-      <c r="E78" s="73"/>
-      <c r="F78" s="73"/>
-      <c r="G78" s="73"/>
-      <c r="H78" s="73"/>
-      <c r="I78" s="73"/>
-      <c r="J78" s="73"/>
-      <c r="K78" s="73"/>
-      <c r="L78" s="73"/>
+      <c r="D78" s="74"/>
+      <c r="E78" s="74"/>
+      <c r="F78" s="74"/>
+      <c r="G78" s="74"/>
+      <c r="H78" s="74"/>
+      <c r="I78" s="74"/>
+      <c r="J78" s="74"/>
+      <c r="K78" s="74"/>
+      <c r="L78" s="74"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B79" s="29" t="s">
@@ -7570,15 +7835,15 @@
       <c r="C79" s="24">
         <v>-0.30588787655775207</v>
       </c>
-      <c r="D79" s="73"/>
-      <c r="E79" s="73"/>
-      <c r="F79" s="73"/>
-      <c r="G79" s="73"/>
-      <c r="H79" s="73"/>
-      <c r="I79" s="73"/>
-      <c r="J79" s="73"/>
-      <c r="K79" s="73"/>
-      <c r="L79" s="73"/>
+      <c r="D79" s="74"/>
+      <c r="E79" s="74"/>
+      <c r="F79" s="74"/>
+      <c r="G79" s="74"/>
+      <c r="H79" s="74"/>
+      <c r="I79" s="74"/>
+      <c r="J79" s="74"/>
+      <c r="K79" s="74"/>
+      <c r="L79" s="74"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B80" s="29" t="s">
@@ -7587,15 +7852,15 @@
       <c r="C80" s="24">
         <v>0.4</v>
       </c>
-      <c r="D80" s="73"/>
-      <c r="E80" s="73"/>
-      <c r="F80" s="73"/>
-      <c r="G80" s="73"/>
-      <c r="H80" s="73"/>
-      <c r="I80" s="73"/>
-      <c r="J80" s="73"/>
-      <c r="K80" s="73"/>
-      <c r="L80" s="73"/>
+      <c r="D80" s="74"/>
+      <c r="E80" s="74"/>
+      <c r="F80" s="74"/>
+      <c r="G80" s="74"/>
+      <c r="H80" s="74"/>
+      <c r="I80" s="74"/>
+      <c r="J80" s="74"/>
+      <c r="K80" s="74"/>
+      <c r="L80" s="74"/>
     </row>
     <row r="81" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B81" s="29" t="s">
@@ -7604,15 +7869,15 @@
       <c r="C81" s="24">
         <v>0.1</v>
       </c>
-      <c r="D81" s="73"/>
-      <c r="E81" s="73"/>
-      <c r="F81" s="73"/>
-      <c r="G81" s="73"/>
-      <c r="H81" s="73"/>
-      <c r="I81" s="73"/>
-      <c r="J81" s="73"/>
-      <c r="K81" s="73"/>
-      <c r="L81" s="73"/>
+      <c r="D81" s="74"/>
+      <c r="E81" s="74"/>
+      <c r="F81" s="74"/>
+      <c r="G81" s="74"/>
+      <c r="H81" s="74"/>
+      <c r="I81" s="74"/>
+      <c r="J81" s="74"/>
+      <c r="K81" s="74"/>
+      <c r="L81" s="74"/>
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B82" s="29" t="s">
@@ -7621,15 +7886,15 @@
       <c r="C82" s="24">
         <v>-0.50785210576888995</v>
       </c>
-      <c r="D82" s="73"/>
-      <c r="E82" s="73"/>
-      <c r="F82" s="73"/>
-      <c r="G82" s="73"/>
-      <c r="H82" s="73"/>
-      <c r="I82" s="73"/>
-      <c r="J82" s="73"/>
-      <c r="K82" s="73"/>
-      <c r="L82" s="73"/>
+      <c r="D82" s="74"/>
+      <c r="E82" s="74"/>
+      <c r="F82" s="74"/>
+      <c r="G82" s="74"/>
+      <c r="H82" s="74"/>
+      <c r="I82" s="74"/>
+      <c r="J82" s="74"/>
+      <c r="K82" s="74"/>
+      <c r="L82" s="74"/>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B83" s="29" t="s">
@@ -7638,15 +7903,15 @@
       <c r="C83" s="24">
         <v>0.19411212344224793</v>
       </c>
-      <c r="D83" s="73"/>
-      <c r="E83" s="73"/>
-      <c r="F83" s="73"/>
-      <c r="G83" s="73"/>
-      <c r="H83" s="73"/>
-      <c r="I83" s="73"/>
-      <c r="J83" s="73"/>
-      <c r="K83" s="73"/>
-      <c r="L83" s="73"/>
+      <c r="D83" s="74"/>
+      <c r="E83" s="74"/>
+      <c r="F83" s="74"/>
+      <c r="G83" s="74"/>
+      <c r="H83" s="74"/>
+      <c r="I83" s="74"/>
+      <c r="J83" s="74"/>
+      <c r="K83" s="74"/>
+      <c r="L83" s="74"/>
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B84" s="29" t="s">
@@ -7655,15 +7920,15 @@
       <c r="C84" s="24">
         <v>-0.26082884634154524</v>
       </c>
-      <c r="D84" s="73"/>
-      <c r="E84" s="73"/>
-      <c r="F84" s="73"/>
-      <c r="G84" s="73"/>
-      <c r="H84" s="73"/>
-      <c r="I84" s="73"/>
-      <c r="J84" s="73"/>
-      <c r="K84" s="73"/>
-      <c r="L84" s="73"/>
+      <c r="D84" s="74"/>
+      <c r="E84" s="74"/>
+      <c r="F84" s="74"/>
+      <c r="G84" s="74"/>
+      <c r="H84" s="74"/>
+      <c r="I84" s="74"/>
+      <c r="J84" s="74"/>
+      <c r="K84" s="74"/>
+      <c r="L84" s="74"/>
     </row>
     <row r="85" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B85" s="29" t="s">
@@ -7672,15 +7937,15 @@
       <c r="C85" s="24">
         <v>-0.13802506750700472</v>
       </c>
-      <c r="D85" s="73"/>
-      <c r="E85" s="73"/>
-      <c r="F85" s="73"/>
-      <c r="G85" s="73"/>
-      <c r="H85" s="73"/>
-      <c r="I85" s="73"/>
-      <c r="J85" s="73"/>
-      <c r="K85" s="73"/>
-      <c r="L85" s="73"/>
+      <c r="D85" s="74"/>
+      <c r="E85" s="74"/>
+      <c r="F85" s="74"/>
+      <c r="G85" s="74"/>
+      <c r="H85" s="74"/>
+      <c r="I85" s="74"/>
+      <c r="J85" s="74"/>
+      <c r="K85" s="74"/>
+      <c r="L85" s="74"/>
     </row>
     <row r="86" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B86" s="30" t="s">
@@ -7689,15 +7954,15 @@
       <c r="C86" s="24">
         <v>-0.40785210576888997</v>
       </c>
-      <c r="D86" s="73"/>
-      <c r="E86" s="73"/>
-      <c r="F86" s="73"/>
-      <c r="G86" s="73"/>
-      <c r="H86" s="73"/>
-      <c r="I86" s="73"/>
-      <c r="J86" s="73"/>
-      <c r="K86" s="73"/>
-      <c r="L86" s="73"/>
+      <c r="D86" s="74"/>
+      <c r="E86" s="74"/>
+      <c r="F86" s="74"/>
+      <c r="G86" s="74"/>
+      <c r="H86" s="74"/>
+      <c r="I86" s="74"/>
+      <c r="J86" s="74"/>
+      <c r="K86" s="74"/>
+      <c r="L86" s="74"/>
     </row>
     <row r="87" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B87" s="30" t="s">
@@ -7706,15 +7971,15 @@
       <c r="C87" s="24">
         <v>0.19411212344224793</v>
       </c>
-      <c r="D87" s="73"/>
-      <c r="E87" s="73"/>
-      <c r="F87" s="73"/>
-      <c r="G87" s="73"/>
-      <c r="H87" s="73"/>
-      <c r="I87" s="73"/>
-      <c r="J87" s="73"/>
-      <c r="K87" s="73"/>
-      <c r="L87" s="73"/>
+      <c r="D87" s="74"/>
+      <c r="E87" s="74"/>
+      <c r="F87" s="74"/>
+      <c r="G87" s="74"/>
+      <c r="H87" s="74"/>
+      <c r="I87" s="74"/>
+      <c r="J87" s="74"/>
+      <c r="K87" s="74"/>
+      <c r="L87" s="74"/>
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B88" s="30" t="s">
@@ -7723,18 +7988,52 @@
       <c r="C88" s="24">
         <v>0.21805217039291008</v>
       </c>
-      <c r="D88" s="73"/>
-      <c r="E88" s="73"/>
-      <c r="F88" s="73"/>
-      <c r="G88" s="73"/>
-      <c r="H88" s="73"/>
-      <c r="I88" s="73"/>
-      <c r="J88" s="73"/>
-      <c r="K88" s="73"/>
-      <c r="L88" s="73"/>
+      <c r="D88" s="74"/>
+      <c r="E88" s="74"/>
+      <c r="F88" s="74"/>
+      <c r="G88" s="74"/>
+      <c r="H88" s="74"/>
+      <c r="I88" s="74"/>
+      <c r="J88" s="74"/>
+      <c r="K88" s="74"/>
+      <c r="L88" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="D87:I87"/>
+    <mergeCell ref="J87:L87"/>
+    <mergeCell ref="D88:I88"/>
+    <mergeCell ref="J88:L88"/>
+    <mergeCell ref="D84:I84"/>
+    <mergeCell ref="J84:L84"/>
+    <mergeCell ref="D85:I85"/>
+    <mergeCell ref="J85:L85"/>
+    <mergeCell ref="D86:I86"/>
+    <mergeCell ref="J86:L86"/>
+    <mergeCell ref="D81:I81"/>
+    <mergeCell ref="J81:L81"/>
+    <mergeCell ref="D82:I82"/>
+    <mergeCell ref="J82:L82"/>
+    <mergeCell ref="D83:I83"/>
+    <mergeCell ref="J83:L83"/>
+    <mergeCell ref="D78:I78"/>
+    <mergeCell ref="J78:L78"/>
+    <mergeCell ref="D79:I79"/>
+    <mergeCell ref="J79:L79"/>
+    <mergeCell ref="D80:I80"/>
+    <mergeCell ref="J80:L80"/>
+    <mergeCell ref="D75:I75"/>
+    <mergeCell ref="J75:L75"/>
+    <mergeCell ref="D76:I76"/>
+    <mergeCell ref="J76:L76"/>
+    <mergeCell ref="D77:I77"/>
+    <mergeCell ref="J77:L77"/>
+    <mergeCell ref="C63:I63"/>
+    <mergeCell ref="J63:K63"/>
+    <mergeCell ref="C64:I64"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="D74:I74"/>
+    <mergeCell ref="J74:L74"/>
     <mergeCell ref="C50:G50"/>
     <mergeCell ref="J50:K50"/>
     <mergeCell ref="C62:I62"/>
@@ -7750,40 +8049,6 @@
     <mergeCell ref="J53:K53"/>
     <mergeCell ref="C61:I61"/>
     <mergeCell ref="J61:K61"/>
-    <mergeCell ref="C63:I63"/>
-    <mergeCell ref="J63:K63"/>
-    <mergeCell ref="C64:I64"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="D74:I74"/>
-    <mergeCell ref="J74:L74"/>
-    <mergeCell ref="D75:I75"/>
-    <mergeCell ref="J75:L75"/>
-    <mergeCell ref="D76:I76"/>
-    <mergeCell ref="J76:L76"/>
-    <mergeCell ref="D77:I77"/>
-    <mergeCell ref="J77:L77"/>
-    <mergeCell ref="D78:I78"/>
-    <mergeCell ref="J78:L78"/>
-    <mergeCell ref="D79:I79"/>
-    <mergeCell ref="J79:L79"/>
-    <mergeCell ref="D80:I80"/>
-    <mergeCell ref="J80:L80"/>
-    <mergeCell ref="D81:I81"/>
-    <mergeCell ref="J81:L81"/>
-    <mergeCell ref="D82:I82"/>
-    <mergeCell ref="J82:L82"/>
-    <mergeCell ref="D83:I83"/>
-    <mergeCell ref="J83:L83"/>
-    <mergeCell ref="D87:I87"/>
-    <mergeCell ref="J87:L87"/>
-    <mergeCell ref="D88:I88"/>
-    <mergeCell ref="J88:L88"/>
-    <mergeCell ref="D84:I84"/>
-    <mergeCell ref="J84:L84"/>
-    <mergeCell ref="D85:I85"/>
-    <mergeCell ref="J85:L85"/>
-    <mergeCell ref="D86:I86"/>
-    <mergeCell ref="J86:L86"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7803,7 +8068,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
@@ -7839,7 +8104,7 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G4" t="s">
         <v>204</v>
@@ -7869,16 +8134,16 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B1" t="s">
+        <v>405</v>
+      </c>
+      <c r="C1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D1" t="s">
         <v>403</v>
-      </c>
-      <c r="B1" t="s">
-        <v>406</v>
-      </c>
-      <c r="C1" t="s">
-        <v>405</v>
-      </c>
-      <c r="D1" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -7932,7 +8197,7 @@
         <v>2</v>
       </c>
       <c r="K4" s="24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="L4" s="24" t="s">
         <v>0</v>
@@ -7959,7 +8224,7 @@
       </c>
       <c r="K5" s="24"/>
       <c r="L5" s="24" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="M5" s="24">
         <f>MEDIAN(A2:A26)</f>
@@ -7982,10 +8247,10 @@
         <v>1</v>
       </c>
       <c r="K6" s="24" t="s">
+        <v>394</v>
+      </c>
+      <c r="L6" s="24" t="s">
         <v>395</v>
-      </c>
-      <c r="L6" s="24" t="s">
-        <v>396</v>
       </c>
       <c r="M6" s="24">
         <f>MODE(A2:A26)</f>
@@ -8009,7 +8274,7 @@
       </c>
       <c r="K7" s="24"/>
       <c r="L7" s="68" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="M7" s="68"/>
     </row>
@@ -8029,10 +8294,10 @@
         <v>1</v>
       </c>
       <c r="K8" s="24" t="s">
+        <v>397</v>
+      </c>
+      <c r="L8" s="24" t="s">
         <v>398</v>
-      </c>
-      <c r="L8" s="24" t="s">
-        <v>399</v>
       </c>
       <c r="M8" s="24">
         <f>(MAX(A:A)-MIN(A:A))</f>
@@ -8055,10 +8320,10 @@
         <v>2</v>
       </c>
       <c r="K9" s="24" t="s">
+        <v>399</v>
+      </c>
+      <c r="L9" s="24" t="s">
         <v>400</v>
-      </c>
-      <c r="L9" s="24" t="s">
-        <v>401</v>
       </c>
       <c r="M9" s="24">
         <v>25</v>
@@ -8081,7 +8346,7 @@
       </c>
       <c r="K10" s="24"/>
       <c r="L10" s="24" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="M10" s="24">
         <v>48</v>
@@ -8103,10 +8368,10 @@
         <v>1</v>
       </c>
       <c r="K11" s="24" t="s">
+        <v>406</v>
+      </c>
+      <c r="L11" s="24" t="s">
         <v>407</v>
-      </c>
-      <c r="L11" s="24" t="s">
-        <v>408</v>
       </c>
       <c r="M11" s="24">
         <v>14</v>
@@ -8129,7 +8394,7 @@
       </c>
       <c r="K12" s="24"/>
       <c r="L12" s="24" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="M12" s="24">
         <v>25</v>
@@ -8152,7 +8417,7 @@
       </c>
       <c r="K13" s="24"/>
       <c r="L13" s="24" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="M13" s="24">
         <v>37</v>
@@ -8175,7 +8440,7 @@
       </c>
       <c r="K14" s="24"/>
       <c r="L14" s="24" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="M14" s="24">
         <v>48</v>
@@ -8198,7 +8463,7 @@
       </c>
       <c r="K15" s="24"/>
       <c r="L15" s="24" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="M15" s="24">
         <v>80</v>
@@ -8220,10 +8485,10 @@
         <v>4</v>
       </c>
       <c r="K16" s="24" t="s">
+        <v>409</v>
+      </c>
+      <c r="L16" s="68" t="s">
         <v>410</v>
-      </c>
-      <c r="L16" s="68" t="s">
-        <v>411</v>
       </c>
       <c r="M16" s="68"/>
     </row>
@@ -8446,7 +8711,7 @@
         <v>81</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -8599,7 +8864,7 @@
         <v>35</v>
       </c>
       <c r="B15" s="69" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C15" s="69"/>
       <c r="D15" s="69"/>
@@ -8612,7 +8877,7 @@
         <v>38</v>
       </c>
       <c r="B16" s="69" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C16" s="69"/>
       <c r="D16" s="69"/>
@@ -8645,7 +8910,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H19" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -9359,7 +9624,7 @@
         <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H7">
         <f>SUM(A2:A4)</f>
@@ -9370,7 +9635,7 @@
         <v>16.666666666666668</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -9381,7 +9646,7 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H8">
         <f>SUM(A5:A7)</f>
@@ -9392,7 +9657,7 @@
         <v>22.333333333333332</v>
       </c>
       <c r="J8" s="60" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -9403,7 +9668,7 @@
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H9">
         <f>SUM(A8:A10)</f>
@@ -9414,7 +9679,7 @@
         <v>29.666666666666668</v>
       </c>
       <c r="J9" s="60" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -9425,7 +9690,7 @@
         <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H10">
         <f>SUM(A11:A13)</f>
@@ -9436,7 +9701,7 @@
         <v>34</v>
       </c>
       <c r="J10" s="60" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -9447,7 +9712,7 @@
         <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H11">
         <f>SUM(A14:A16)</f>
@@ -9458,7 +9723,7 @@
         <v>37</v>
       </c>
       <c r="J11" s="60" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -9469,7 +9734,7 @@
         <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H12">
         <f>SUM(A17:A19)</f>
@@ -9480,7 +9745,7 @@
         <v>46</v>
       </c>
       <c r="J12" s="60" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -9491,7 +9756,7 @@
         <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H13">
         <f>SUM(A20:A22)</f>
@@ -9502,7 +9767,7 @@
         <v>48.666666666666664</v>
       </c>
       <c r="J13" s="60" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -9513,7 +9778,7 @@
         <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H14">
         <f>SUM(A23:A25)</f>
@@ -9524,7 +9789,7 @@
         <v>69</v>
       </c>
       <c r="J14" s="60" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -9592,7 +9857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:R152"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
@@ -9632,16 +9897,16 @@
         <v>61</v>
       </c>
       <c r="M2" s="66" t="s">
+        <v>432</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>433</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>435</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -9903,7 +10168,7 @@
         <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="M13" s="66">
         <v>2.4</v>
@@ -10071,7 +10336,7 @@
         <v>54</v>
       </c>
       <c r="E20" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="M20" s="66">
         <v>2.5</v>
@@ -10171,7 +10436,7 @@
         <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="M24" s="66">
         <v>2.6</v>
@@ -10223,7 +10488,7 @@
         <v>0.53</v>
       </c>
       <c r="F26" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="M26" s="66">
         <v>2.6</v>
@@ -10352,7 +10617,7 @@
         <v>56</v>
       </c>
       <c r="F32" s="59" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="M32" s="66">
         <v>2.7</v>
@@ -10378,7 +10643,7 @@
         <v>57</v>
       </c>
       <c r="F33" s="67" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="M33" s="66">
         <v>2.7</v>
@@ -10404,7 +10669,7 @@
         <v>58</v>
       </c>
       <c r="F34" s="59" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="M34" s="66">
         <v>2.7</v>
@@ -12439,19 +12704,21 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD9730A-8100-48F4-8E66-D519E6FB08E9}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="3.42578125" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="4" customWidth="1"/>
     <col min="13" max="13" width="3.42578125" customWidth="1"/>
   </cols>
@@ -12468,7 +12735,7 @@
     </row>
     <row r="3" spans="1:9" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="70" t="s">
-        <v>228</v>
+        <v>439</v>
       </c>
       <c r="D3" s="70"/>
       <c r="E3" s="70"/>
@@ -12479,12 +12746,17 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>230</v>
+        <v>229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -12492,31 +12764,31 @@
         <v>227</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
+        <v>231</v>
+      </c>
+      <c r="E10" t="s">
         <v>232</v>
-      </c>
-      <c r="E10" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
+        <v>233</v>
+      </c>
+      <c r="E11" t="s">
         <v>234</v>
-      </c>
-      <c r="E11" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
+        <v>235</v>
+      </c>
+      <c r="E12" t="s">
         <v>236</v>
-      </c>
-      <c r="E12" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -12526,40 +12798,40 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>89</v>
       </c>
@@ -12567,15 +12839,327 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>92</v>
       </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="77" t="s">
+        <v>442</v>
+      </c>
+      <c r="H32" s="77" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="76" t="s">
+        <v>231</v>
+      </c>
+      <c r="H33" s="76" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="76" t="s">
+        <v>233</v>
+      </c>
+      <c r="E34" s="77" t="s">
+        <v>445</v>
+      </c>
+      <c r="H34" s="76" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>446</v>
+      </c>
+      <c r="H35" s="76" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E36" s="24" t="s">
+        <v>447</v>
+      </c>
+      <c r="H36" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E37" s="77" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="77" t="s">
+        <v>443</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="76" t="s">
+        <v>238</v>
+      </c>
+      <c r="E39" s="24" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C40" s="76" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C41" s="76" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C42" s="76" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C43" s="76" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C44" s="21" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="34"/>
+      <c r="B47" s="34"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="34"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="34"/>
+      <c r="G47" s="34"/>
+      <c r="H47" s="34"/>
+      <c r="I47" s="34"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="34"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="34"/>
+      <c r="G48" s="34"/>
+      <c r="H48" s="34"/>
+      <c r="I48" s="34"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="34"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="34"/>
+      <c r="D49" s="34"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="34"/>
+      <c r="G49" s="34"/>
+      <c r="H49" s="34"/>
+      <c r="I49" s="34"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="34"/>
+      <c r="B50" s="34"/>
+      <c r="C50" s="34"/>
+      <c r="D50" s="34"/>
+      <c r="E50" s="34"/>
+      <c r="F50" s="34"/>
+      <c r="G50" s="34"/>
+      <c r="H50" s="34"/>
+      <c r="I50" s="34"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="34"/>
+      <c r="B51" s="34"/>
+      <c r="C51" s="34"/>
+      <c r="D51" s="34"/>
+      <c r="E51" s="34"/>
+      <c r="F51" s="34"/>
+      <c r="G51" s="34"/>
+      <c r="H51" s="34"/>
+      <c r="I51" s="34"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="34"/>
+      <c r="B52" s="34"/>
+      <c r="C52" s="34"/>
+      <c r="D52" s="34"/>
+      <c r="E52" s="34"/>
+      <c r="F52" s="34"/>
+      <c r="G52" s="34"/>
+      <c r="H52" s="34"/>
+      <c r="I52" s="34"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="34"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="34"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="34"/>
+      <c r="G53" s="34"/>
+      <c r="H53" s="34"/>
+      <c r="I53" s="34"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="34"/>
+      <c r="B54" s="34"/>
+      <c r="C54" s="34"/>
+      <c r="D54" s="34"/>
+      <c r="E54" s="34"/>
+      <c r="F54" s="34"/>
+      <c r="G54" s="34"/>
+      <c r="H54" s="34"/>
+      <c r="I54" s="34"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="34"/>
+      <c r="B55" s="34"/>
+      <c r="C55" s="34"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="34"/>
+      <c r="G55" s="34"/>
+      <c r="H55" s="34"/>
+      <c r="I55" s="34"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="34"/>
+      <c r="B56" s="34"/>
+      <c r="C56" s="34"/>
+      <c r="D56" s="34"/>
+      <c r="E56" s="34"/>
+      <c r="F56" s="34"/>
+      <c r="G56" s="34"/>
+      <c r="H56" s="34"/>
+      <c r="I56" s="34"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="34"/>
+      <c r="B57" s="34"/>
+      <c r="C57" s="34"/>
+      <c r="D57" s="34"/>
+      <c r="E57" s="34"/>
+      <c r="F57" s="34"/>
+      <c r="G57" s="34"/>
+      <c r="H57" s="34"/>
+      <c r="I57" s="34"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="34"/>
+      <c r="B58" s="34"/>
+      <c r="C58" s="34"/>
+      <c r="D58" s="34"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="34"/>
+      <c r="G58" s="34"/>
+      <c r="H58" s="34"/>
+      <c r="I58" s="34"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="34"/>
+      <c r="B59" s="34"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="34"/>
+      <c r="E59" s="34"/>
+      <c r="F59" s="34"/>
+      <c r="G59" s="34"/>
+      <c r="H59" s="34"/>
+      <c r="I59" s="34"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="34"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="34"/>
+      <c r="D60" s="34"/>
+      <c r="E60" s="34"/>
+      <c r="F60" s="34"/>
+      <c r="G60" s="34"/>
+      <c r="H60" s="34"/>
+      <c r="I60" s="34"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="34"/>
+      <c r="B61" s="34"/>
+      <c r="C61" s="34"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="34"/>
+      <c r="F61" s="34"/>
+      <c r="G61" s="34"/>
+      <c r="H61" s="34"/>
+      <c r="I61" s="34"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="34"/>
+      <c r="B62" s="34"/>
+      <c r="C62" s="34"/>
+      <c r="D62" s="34"/>
+      <c r="E62" s="34"/>
+      <c r="F62" s="34"/>
+      <c r="G62" s="34"/>
+      <c r="H62" s="34"/>
+      <c r="I62" s="34"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="34"/>
+      <c r="B63" s="34"/>
+      <c r="C63" s="34"/>
+      <c r="D63" s="34"/>
+      <c r="E63" s="34"/>
+      <c r="F63" s="34"/>
+      <c r="G63" s="34"/>
+      <c r="H63" s="34"/>
+      <c r="I63" s="34"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="34"/>
+      <c r="B64" s="34"/>
+      <c r="C64" s="34"/>
+      <c r="D64" s="34"/>
+      <c r="E64" s="34"/>
+      <c r="F64" s="34"/>
+      <c r="G64" s="34"/>
+      <c r="H64" s="34"/>
+      <c r="I64" s="34"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="34"/>
+      <c r="B65" s="34"/>
+      <c r="C65" s="34"/>
+      <c r="D65" s="34"/>
+      <c r="E65" s="34"/>
+      <c r="F65" s="34"/>
+      <c r="G65" s="34"/>
+      <c r="H65" s="34"/>
+      <c r="I65" s="34"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="34"/>
+      <c r="B66" s="34"/>
+      <c r="C66" s="34"/>
+      <c r="D66" s="34"/>
+      <c r="E66" s="34"/>
+      <c r="F66" s="34"/>
+      <c r="G66" s="34"/>
+      <c r="H66" s="34"/>
+      <c r="I66" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -12583,21 +13167,23 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="94" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39ABA2D1-388C-4218-8BE1-29873196265A}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="4.42578125" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
@@ -12617,91 +13203,148 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>41</v>
       </c>
       <c r="B33" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+      <c r="K33" t="s">
+        <v>454</v>
+      </c>
+      <c r="L33" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>41</v>
       </c>
       <c r="B34" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+        <v>245</v>
+      </c>
+      <c r="K34" t="s">
+        <v>454</v>
+      </c>
+      <c r="L34" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="35" t="s">
         <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+        <v>246</v>
+      </c>
+      <c r="K35" t="s">
+        <v>454</v>
+      </c>
+      <c r="L35" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="35" t="s">
         <v>41</v>
       </c>
       <c r="B36" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+        <v>247</v>
+      </c>
+      <c r="K36" t="s">
+        <v>454</v>
+      </c>
+      <c r="L36" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="35" t="s">
         <v>41</v>
       </c>
       <c r="B37" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+        <v>248</v>
+      </c>
+      <c r="K37" t="s">
+        <v>454</v>
+      </c>
+      <c r="L37" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="35" t="s">
         <v>41</v>
       </c>
       <c r="B38" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K38" t="s">
+        <v>454</v>
+      </c>
+      <c r="L38" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="35" t="s">
         <v>41</v>
       </c>
       <c r="B39" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K39" t="s">
+        <v>454</v>
+      </c>
+      <c r="L39" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="35" t="s">
         <v>41</v>
       </c>
       <c r="B40" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="K40" t="s">
+        <v>454</v>
+      </c>
+      <c r="L40" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>391</v>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>458</v>
+      </c>
+      <c r="C46">
+        <f xml:space="preserve"> (3+1)*(3+1)+(6+1)*(3+1)</f>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -12726,22 +13369,22 @@
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -12751,32 +13394,32 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -12791,7 +13434,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -12822,7 +13465,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>